<commit_message>
support action param 6 & dynamic height
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D807AAC-6B54-43DA-98C3-44D67354A0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD6473F-8663-4568-B435-A8F8424DFA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4010" yWindow="3660" windowWidth="29710" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="1054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="1055">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3194,6 +3194,10 @@
   </si>
   <si>
     <t>ObjectFilterTitle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerParameter#6value</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3570,7 +3574,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B555"/>
+  <dimension ref="A1:B556"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A549" workbookViewId="0">
       <selection activeCell="B556" sqref="B556"/>
@@ -7991,7 +7995,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="554" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A554" s="4" t="s">
         <v>1052</v>
       </c>
@@ -7999,12 +8003,17 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="555" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A555" s="4" t="s">
         <v>1051</v>
       </c>
       <c r="B555" s="3" t="s">
         <v>1050</v>
+      </c>
+    </row>
+    <row r="556" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A556" s="1" t="s">
+        <v>1054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tileset multiselection button
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD6473F-8663-4568-B435-A8F8424DFA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E739DF44-354E-4561-A51A-4682448F01BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4010" yWindow="3660" windowWidth="29710" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="1059">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3198,6 +3198,20 @@
   </si>
   <si>
     <t>TriggerParameter#6value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultiSelectionTileSetAdd</t>
+  </si>
+  <si>
+    <t>同类添加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultiSelectionTileSetDelete</t>
+  </si>
+  <si>
+    <t>同类删除</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3574,10 +3588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B556"/>
+  <dimension ref="A1:B558"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A549" workbookViewId="0">
-      <selection activeCell="B556" sqref="B556"/>
+    <sheetView tabSelected="1" topLeftCell="A548" workbookViewId="0">
+      <selection activeCell="B558" sqref="A557:B558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8016,6 +8030,22 @@
         <v>1054</v>
       </c>
     </row>
+    <row r="557" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A557" s="4" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B557" s="3" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A558" s="4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B558" s="3" t="s">
+        <v>1058</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add AddOre and ReduceOre button
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E739DF44-354E-4561-A51A-4682448F01BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59744275-800C-49A2-A489-0A9A783F8723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4010" yWindow="3660" windowWidth="29710" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="2120" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="1063">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3212,6 +3212,22 @@
   </si>
   <si>
     <t>同类删除</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddOreObList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReduceOreObList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>减少矿石</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加矿石</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3588,10 +3604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B558"/>
+  <dimension ref="A1:B560"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A548" workbookViewId="0">
-      <selection activeCell="B558" sqref="A557:B558"/>
+      <selection activeCell="B559" sqref="B559"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8046,6 +8062,22 @@
         <v>1058</v>
       </c>
     </row>
+    <row r="559" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A559" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B559" s="3" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A560" s="4" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B560" s="3" t="s">
+        <v>1061</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support building shadow display
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59744275-800C-49A2-A489-0A9A783F8723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A00EEAF-FF3F-4EE2-A5B3-0E099C8CB432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="2120" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="1065">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3228,6 +3228,14 @@
   </si>
   <si>
     <t>增加矿石</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.Display.Shadows</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>阴影\tAlt+7</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3604,10 +3612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B560"/>
+  <dimension ref="A1:B561"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A548" workbookViewId="0">
-      <selection activeCell="B559" sqref="B559"/>
+      <selection activeCell="B561" sqref="B561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8078,6 +8086,14 @@
         <v>1061</v>
       </c>
     </row>
+    <row r="561" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A561" s="4" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B561" s="3" t="s">
+        <v>1064</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support alphaimage for building & terrain
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A00EEAF-FF3F-4EE2-A5B3-0E099C8CB432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E0328F-6754-4AF5-915A-AF9B19A4E4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="2120" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3179,12 +3179,6 @@
     <t>对象筛选</t>
   </si>
   <si>
-    <t>请输入对象ID:\n\n多个对象使用\",\"分隔，留空以显示所有对象。\n确认后，设置对象属性筛选（可选）。</t>
-  </si>
-  <si>
-    <t>请输入单元标记ID:\n\n多个单元标记使用\",\"分隔。可以只输入ID最后的数字。</t>
-  </si>
-  <si>
     <t>ObjectFilterMessageCT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3236,6 +3230,14 @@
   </si>
   <si>
     <t>阴影\tAlt+7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>请输入对象ID:\n\n多个对象使用","分隔，留空以显示所有对象。\n确认后，设置对象属性筛选（可选）。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>请输入单元标记ID:\n\n多个单元标记使用","分隔。可以只输入ID最后的数字。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3615,7 +3617,7 @@
   <dimension ref="A1:B561"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A548" workbookViewId="0">
-      <selection activeCell="B561" sqref="B561"/>
+      <selection activeCell="C554" sqref="C554"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8027,7 +8029,7 @@
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A553" s="4" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B553" s="3" t="s">
         <v>1048</v>
@@ -8035,63 +8037,63 @@
     </row>
     <row r="554" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A554" s="4" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="B554" s="3" t="s">
-        <v>1049</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A555" s="4" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1050</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A556" s="1" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A557" s="4" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="B557" s="3" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A558" s="4" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="B558" s="3" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A559" s="4" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="B559" s="3" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A560" s="4" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="B560" s="3" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A561" s="4" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="B561" s="3" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add extconfigs, rewrite basenode drawing
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E0328F-6754-4AF5-915A-AF9B19A4E4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5B25E0-B149-4F5E-8ED2-1302C9E75B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="2120" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="1067">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3238,6 +3238,14 @@
   </si>
   <si>
     <t>请输入单元标记ID:\n\n多个单元标记使用","分隔。可以只输入ID最后的数字。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.Display.AlphaImages</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alpha光\tAlt+8</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3614,10 +3622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B561"/>
+  <dimension ref="A1:B562"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A548" workbookViewId="0">
-      <selection activeCell="C554" sqref="C554"/>
+      <selection activeCell="B560" sqref="B560"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8096,6 +8104,14 @@
         <v>1062</v>
       </c>
     </row>
+    <row r="562" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A562" s="4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B562" s="3" t="s">
+        <v>1066</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support include in map file
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5B25E0-B149-4F5E-8ED2-1302C9E75B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A9352B-7143-4FF8-9D98-739C0685CD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="2120" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="1069">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3246,6 +3257,14 @@
   </si>
   <si>
     <t>Alpha光\tAlt+8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapIncludeWarningMessage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>此地图包含include INI,所有INI中的键值对既不会被保存到地图内,也不会保存到INI中。\n点击“确定”,此地图将不再弹出警告。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3622,10 +3641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B562"/>
+  <dimension ref="A1:B563"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A548" workbookViewId="0">
-      <selection activeCell="B560" sqref="B560"/>
+      <selection activeCell="B563" sqref="B563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8112,6 +8131,14 @@
         <v>1066</v>
       </c>
     </row>
+    <row r="563" spans="1:2" ht="52.5" x14ac:dyDescent="0.3">
+      <c r="A563" s="4" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B563" s="3" t="s">
+        <v>1068</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support double click select csf
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A9352B-7143-4FF8-9D98-739C0685CD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86420EE1-604F-4997-9986-9A46F79C885F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="2120" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -767,9 +767,6 @@
     <t>CsfEditorDescription1</t>
   </si>
   <si>
-    <t>当触发编辑器启动，且选中行为的参数中有CSF文本时，点击“应用”以应用当前选中的CSF文本。</t>
-  </si>
-  <si>
     <t>CsfEditorDescription2</t>
   </si>
   <si>
@@ -3265,6 +3262,10 @@
   </si>
   <si>
     <t>此地图包含include INI,所有INI中的键值对既不会被保存到地图内,也不会保存到INI中。\n点击“确定”,此地图将不再弹出警告。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>当触发编辑器启动，且选中行为的参数中有CSF文本时，点击“应用”或双击当前项以应用当前选中的CSF文本。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3643,8 +3644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B563"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A548" workbookViewId="0">
-      <selection activeCell="B563" sqref="B563"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -3655,10 +3656,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1041</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1042</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" thickTop="1" x14ac:dyDescent="0.3">
@@ -4715,1220 +4716,1220 @@
         <v>242</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>243</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="52.5" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B150" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B157" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B160" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B161" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B162" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B163" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B181" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B182" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B183" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B184" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B188" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B189" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B190" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B191" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B192" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B193" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B197" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>368</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B199" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B200" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B201" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="B201" s="2" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B202" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B202" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B203" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="B203" s="2" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B204" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="B204" s="2" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B206" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B207" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="B207" s="2" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B209" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B210" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B211" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B212" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>398</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B214" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B215" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B216" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="B216" s="2" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B217" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="B217" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B219" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="B219" s="2" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B220" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="B221" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B222" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="B222" s="2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B224" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="B224" s="2" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B225" s="2" t="s">
         <v>422</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B227" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="B227" s="2" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B228" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="B228" s="2" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B229" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="B229" s="2" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B230" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B231" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="B231" s="2" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B232" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="B232" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B233" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B234" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B235" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="B235" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B236" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B237" s="2" t="s">
         <v>446</v>
-      </c>
-      <c r="B237" s="2" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B238" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="B238" s="2" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B239" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="B239" s="2" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B240" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="B240" s="2" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B241" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="B241" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B242" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="B242" s="2" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B243" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="B243" s="2" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B244" s="2" t="s">
         <v>460</v>
-      </c>
-      <c r="B244" s="2" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B245" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="B245" s="2" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B246" s="2" t="s">
         <v>464</v>
-      </c>
-      <c r="B246" s="2" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B247" s="2" t="s">
         <v>466</v>
-      </c>
-      <c r="B247" s="2" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B248" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="B248" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B249" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="B249" s="2" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B250" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="B250" s="2" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B251" s="2" t="s">
         <v>474</v>
-      </c>
-      <c r="B251" s="2" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B252" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="B252" s="2" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B253" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="B253" s="2" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B254" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="B254" s="2" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B255" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="B255" s="2" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B256" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="B256" s="2" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B257" s="2" t="s">
         <v>486</v>
-      </c>
-      <c r="B257" s="2" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B258" s="2" t="s">
         <v>488</v>
-      </c>
-      <c r="B258" s="2" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B259" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="B259" s="2" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B260" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="B260" s="2" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B261" s="2" t="s">
         <v>494</v>
-      </c>
-      <c r="B261" s="2" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B262" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="B262" s="2" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B263" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="B263" s="2" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B264" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="B264" s="2" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B265" s="2" t="s">
         <v>502</v>
-      </c>
-      <c r="B265" s="2" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B266" s="2" t="s">
         <v>504</v>
-      </c>
-      <c r="B266" s="2" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B267" s="2" t="s">
         <v>506</v>
-      </c>
-      <c r="B267" s="2" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B268" s="2" t="s">
         <v>508</v>
-      </c>
-      <c r="B268" s="2" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B269" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="B269" s="2" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B270" s="2" t="s">
         <v>512</v>
-      </c>
-      <c r="B270" s="2" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B271" s="2" t="s">
         <v>514</v>
-      </c>
-      <c r="B271" s="2" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B272" s="2" t="s">
         <v>516</v>
-      </c>
-      <c r="B272" s="2" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B273" s="2" t="s">
         <v>518</v>
-      </c>
-      <c r="B273" s="2" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B274" s="2" t="s">
         <v>520</v>
-      </c>
-      <c r="B274" s="2" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B275" s="2" t="s">
         <v>522</v>
-      </c>
-      <c r="B275" s="2" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B276" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="B276" s="2" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B277" s="2" t="s">
         <v>526</v>
-      </c>
-      <c r="B277" s="2" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B278" s="2" t="s">
         <v>528</v>
-      </c>
-      <c r="B278" s="2" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B279" s="2" t="s">
         <v>530</v>
-      </c>
-      <c r="B279" s="2" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B280" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="B280" s="2" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B281" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="B281" s="2" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B282" s="2" t="s">
         <v>536</v>
-      </c>
-      <c r="B282" s="2" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B283" s="2" t="s">
         <v>538</v>
-      </c>
-      <c r="B283" s="2" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B286" s="2" t="s">
         <v>542</v>
-      </c>
-      <c r="B286" s="2" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>144</v>
@@ -5936,63 +5937,63 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B288" s="2" t="s">
         <v>545</v>
-      </c>
-      <c r="B288" s="2" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B289" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="B289" s="2" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B290" s="2" t="s">
         <v>549</v>
-      </c>
-      <c r="B290" s="2" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B292" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="B292" s="2" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B294" s="2" t="s">
         <v>555</v>
-      </c>
-      <c r="B294" s="2" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>108</v>
@@ -6000,39 +6001,39 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B296" s="2" t="s">
         <v>558</v>
-      </c>
-      <c r="B296" s="2" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="B297" s="2" t="s">
         <v>560</v>
-      </c>
-      <c r="B297" s="2" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B298" s="2" t="s">
         <v>562</v>
-      </c>
-      <c r="B298" s="2" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B299" s="2" t="s">
         <v>564</v>
-      </c>
-      <c r="B299" s="2" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>31</v>
@@ -6040,31 +6041,31 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B301" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="B301" s="2" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B302" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="B302" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B303" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="B303" s="2" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>165</v>
@@ -6072,263 +6073,263 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B305" s="2" t="s">
         <v>574</v>
-      </c>
-      <c r="B305" s="2" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B306" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="B306" s="2" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B310" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="B310" s="2" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B311" s="2" t="s">
         <v>583</v>
-      </c>
-      <c r="B311" s="2" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B312" s="2" t="s">
         <v>585</v>
-      </c>
-      <c r="B312" s="2" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="313" spans="1:2" ht="105" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B313" s="2" t="s">
         <v>587</v>
-      </c>
-      <c r="B313" s="2" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B314" s="2" t="s">
         <v>589</v>
-      </c>
-      <c r="B314" s="2" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B315" s="2" t="s">
         <v>591</v>
-      </c>
-      <c r="B315" s="2" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B316" s="2" t="s">
         <v>593</v>
-      </c>
-      <c r="B316" s="2" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B317" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="B317" s="2" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B318" s="2" t="s">
         <v>597</v>
-      </c>
-      <c r="B318" s="2" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B319" s="2" t="s">
         <v>599</v>
-      </c>
-      <c r="B319" s="2" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B320" s="2" t="s">
         <v>601</v>
-      </c>
-      <c r="B320" s="2" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B321" s="2" t="s">
         <v>603</v>
-      </c>
-      <c r="B321" s="2" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B322" s="2" t="s">
         <v>605</v>
-      </c>
-      <c r="B322" s="2" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B323" s="2" t="s">
         <v>607</v>
-      </c>
-      <c r="B323" s="2" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B324" s="2" t="s">
         <v>609</v>
-      </c>
-      <c r="B324" s="2" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="B325" s="2" t="s">
         <v>611</v>
-      </c>
-      <c r="B325" s="2" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B326" s="2" t="s">
         <v>613</v>
-      </c>
-      <c r="B326" s="2" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B327" s="2" t="s">
         <v>615</v>
-      </c>
-      <c r="B327" s="2" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B328" s="2" t="s">
         <v>617</v>
-      </c>
-      <c r="B328" s="2" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B329" s="2" t="s">
         <v>619</v>
-      </c>
-      <c r="B329" s="2" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B330" s="2" t="s">
         <v>621</v>
-      </c>
-      <c r="B330" s="2" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B331" s="2" t="s">
         <v>623</v>
-      </c>
-      <c r="B331" s="2" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B332" s="2" t="s">
         <v>625</v>
-      </c>
-      <c r="B332" s="2" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B333" s="2" t="s">
         <v>627</v>
-      </c>
-      <c r="B333" s="2" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B334" s="2" t="s">
         <v>629</v>
-      </c>
-      <c r="B334" s="2" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="B335" s="2" t="s">
         <v>631</v>
-      </c>
-      <c r="B335" s="2" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B336" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="B336" s="2" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B337" s="2" t="s">
         <v>67</v>
@@ -6336,7 +6337,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>69</v>
@@ -6344,23 +6345,23 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B339" s="2" t="s">
         <v>637</v>
-      </c>
-      <c r="B339" s="2" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B340" s="2" t="s">
         <v>639</v>
-      </c>
-      <c r="B340" s="2" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>7</v>
@@ -6368,15 +6369,15 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B342" s="2" t="s">
         <v>642</v>
-      </c>
-      <c r="B342" s="2" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A343" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B343" s="2" t="s">
         <v>241</v>
@@ -6384,1023 +6385,1023 @@
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B344" s="2" t="s">
         <v>645</v>
-      </c>
-      <c r="B344" s="2" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B345" s="2" t="s">
         <v>647</v>
-      </c>
-      <c r="B345" s="2" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A346" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B346" s="2" t="s">
         <v>649</v>
-      </c>
-      <c r="B346" s="2" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A347" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B347" s="2" t="s">
         <v>651</v>
-      </c>
-      <c r="B347" s="2" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B348" s="2" t="s">
         <v>653</v>
-      </c>
-      <c r="B348" s="2" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A349" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B349" s="2" t="s">
         <v>655</v>
-      </c>
-      <c r="B349" s="2" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B350" s="2" t="s">
         <v>657</v>
-      </c>
-      <c r="B350" s="2" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="B351" s="2" t="s">
         <v>659</v>
-      </c>
-      <c r="B351" s="2" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="B352" s="2" t="s">
         <v>661</v>
-      </c>
-      <c r="B352" s="2" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B353" s="2" t="s">
         <v>663</v>
-      </c>
-      <c r="B353" s="2" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="B354" s="2" t="s">
         <v>665</v>
-      </c>
-      <c r="B354" s="2" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="B355" s="2" t="s">
         <v>667</v>
-      </c>
-      <c r="B355" s="2" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="B357" s="2" t="s">
         <v>670</v>
-      </c>
-      <c r="B357" s="2" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="358" spans="1:2" ht="70" x14ac:dyDescent="0.3">
       <c r="A358" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="B358" s="2" t="s">
         <v>672</v>
-      </c>
-      <c r="B358" s="2" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B360" s="2" t="s">
         <v>675</v>
-      </c>
-      <c r="B360" s="2" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="361" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="B361" s="2" t="s">
         <v>677</v>
-      </c>
-      <c r="B361" s="2" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="B362" s="2" t="s">
         <v>679</v>
-      </c>
-      <c r="B362" s="2" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="B363" s="2" t="s">
         <v>681</v>
-      </c>
-      <c r="B363" s="2" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="B364" s="2" t="s">
         <v>683</v>
-      </c>
-      <c r="B364" s="2" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B365" s="2" t="s">
         <v>685</v>
-      </c>
-      <c r="B365" s="2" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="366" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="B366" s="2" t="s">
         <v>687</v>
-      </c>
-      <c r="B366" s="2" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="367" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A367" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="B367" s="2" t="s">
         <v>689</v>
-      </c>
-      <c r="B367" s="2" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="B368" s="2" t="s">
         <v>691</v>
-      </c>
-      <c r="B368" s="2" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B369" s="2" t="s">
         <v>693</v>
-      </c>
-      <c r="B369" s="2" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B370" s="2" t="s">
         <v>695</v>
-      </c>
-      <c r="B370" s="2" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="371" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B371" s="2" t="s">
         <v>697</v>
-      </c>
-      <c r="B371" s="2" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B372" s="2" t="s">
         <v>699</v>
-      </c>
-      <c r="B372" s="2" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="B373" s="2" t="s">
         <v>701</v>
-      </c>
-      <c r="B373" s="2" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="B374" s="2" t="s">
         <v>703</v>
-      </c>
-      <c r="B374" s="2" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B375" s="2" t="s">
         <v>705</v>
-      </c>
-      <c r="B375" s="2" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="B376" s="2" t="s">
         <v>707</v>
-      </c>
-      <c r="B376" s="2" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="B377" s="2" t="s">
         <v>709</v>
-      </c>
-      <c r="B377" s="2" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="B378" s="2" t="s">
         <v>711</v>
-      </c>
-      <c r="B378" s="2" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A379" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B379" s="2" t="s">
         <v>713</v>
-      </c>
-      <c r="B379" s="2" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="B380" s="2" t="s">
         <v>715</v>
-      </c>
-      <c r="B380" s="2" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A381" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="B381" s="2" t="s">
         <v>717</v>
-      </c>
-      <c r="B381" s="2" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B382" s="2" t="s">
         <v>719</v>
-      </c>
-      <c r="B382" s="2" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A383" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="B383" s="2" t="s">
         <v>721</v>
-      </c>
-      <c r="B383" s="2" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B384" s="2" t="s">
         <v>723</v>
-      </c>
-      <c r="B384" s="2" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B385" s="2" t="s">
         <v>725</v>
-      </c>
-      <c r="B385" s="2" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="B386" s="2" t="s">
         <v>727</v>
-      </c>
-      <c r="B386" s="2" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B387" s="2" t="s">
         <v>729</v>
-      </c>
-      <c r="B387" s="2" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="B388" s="2" t="s">
         <v>731</v>
-      </c>
-      <c r="B388" s="2" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="B389" s="2" t="s">
         <v>733</v>
-      </c>
-      <c r="B389" s="2" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B390" s="2" t="s">
         <v>735</v>
-      </c>
-      <c r="B390" s="2" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B391" s="2" t="s">
         <v>737</v>
-      </c>
-      <c r="B391" s="2" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="B392" s="2" t="s">
         <v>739</v>
-      </c>
-      <c r="B392" s="2" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="B397" s="2" t="s">
         <v>745</v>
-      </c>
-      <c r="B397" s="2" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B398" s="2" t="s">
         <v>747</v>
-      </c>
-      <c r="B398" s="2" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B399" s="2" t="s">
         <v>749</v>
-      </c>
-      <c r="B399" s="2" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A401" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A402" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B403" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B404" s="2" t="s">
         <v>755</v>
-      </c>
-      <c r="B404" s="2" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B405" s="2" t="s">
         <v>757</v>
-      </c>
-      <c r="B405" s="2" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B406" s="2" t="s">
         <v>759</v>
-      </c>
-      <c r="B406" s="2" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B407" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B408" s="2" t="s">
         <v>762</v>
-      </c>
-      <c r="B408" s="2" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A409" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B409" s="2" t="s">
         <v>764</v>
-      </c>
-      <c r="B409" s="2" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A410" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B410" s="2" t="s">
         <v>766</v>
-      </c>
-      <c r="B410" s="2" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A411" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B411" s="2" t="s">
         <v>768</v>
-      </c>
-      <c r="B411" s="2" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A412" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B412" s="2" t="s">
         <v>770</v>
-      </c>
-      <c r="B412" s="2" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A413" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="B413" s="2" t="s">
         <v>772</v>
-      </c>
-      <c r="B413" s="2" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A414" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B414" s="2" t="s">
         <v>774</v>
-      </c>
-      <c r="B414" s="2" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A415" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B415" s="2" t="s">
         <v>776</v>
-      </c>
-      <c r="B415" s="2" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A416" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B416" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A417" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B417" s="2" t="s">
         <v>779</v>
-      </c>
-      <c r="B417" s="2" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A418" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B418" s="2" t="s">
         <v>781</v>
-      </c>
-      <c r="B418" s="2" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A419" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B419" s="2" t="s">
         <v>783</v>
-      </c>
-      <c r="B419" s="2" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A420" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B420" s="2" t="s">
         <v>785</v>
-      </c>
-      <c r="B420" s="2" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B421" s="2" t="s">
         <v>787</v>
-      </c>
-      <c r="B421" s="2" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A422" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B422" s="2" t="s">
         <v>789</v>
-      </c>
-      <c r="B422" s="2" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A423" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B423" s="2" t="s">
         <v>791</v>
-      </c>
-      <c r="B423" s="2" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A424" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B424" s="2" t="s">
         <v>793</v>
-      </c>
-      <c r="B424" s="2" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A425" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B425" s="2" t="s">
         <v>795</v>
-      </c>
-      <c r="B425" s="2" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A426" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B426" s="2" t="s">
         <v>797</v>
-      </c>
-      <c r="B426" s="2" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A427" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B427" s="2" t="s">
         <v>799</v>
-      </c>
-      <c r="B427" s="2" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A428" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="B428" s="2" t="s">
         <v>801</v>
-      </c>
-      <c r="B428" s="2" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A429" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="B429" s="2" t="s">
         <v>803</v>
-      </c>
-      <c r="B429" s="2" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A430" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B430" s="2" t="s">
         <v>805</v>
-      </c>
-      <c r="B430" s="2" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A431" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B431" s="2" t="s">
         <v>807</v>
-      </c>
-      <c r="B431" s="2" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A432" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B432" s="2" t="s">
         <v>809</v>
-      </c>
-      <c r="B432" s="2" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A433" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B433" s="2" t="s">
         <v>811</v>
-      </c>
-      <c r="B433" s="2" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A434" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B434" s="2" t="s">
         <v>813</v>
-      </c>
-      <c r="B434" s="2" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A435" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="B435" s="2" t="s">
         <v>815</v>
-      </c>
-      <c r="B435" s="2" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A436" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B436" s="2" t="s">
         <v>817</v>
-      </c>
-      <c r="B436" s="2" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A437" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B437" s="2" t="s">
         <v>819</v>
-      </c>
-      <c r="B437" s="2" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A438" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B438" s="2" t="s">
         <v>821</v>
-      </c>
-      <c r="B438" s="2" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B439" s="2" t="s">
         <v>823</v>
-      </c>
-      <c r="B439" s="2" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A440" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B440" s="2" t="s">
         <v>825</v>
-      </c>
-      <c r="B440" s="2" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A441" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="B441" s="2" t="s">
         <v>827</v>
-      </c>
-      <c r="B441" s="2" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B442" s="2" t="s">
         <v>829</v>
-      </c>
-      <c r="B442" s="2" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A443" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B443" s="2" t="s">
         <v>831</v>
-      </c>
-      <c r="B443" s="2" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A444" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="B444" s="2" t="s">
         <v>833</v>
-      </c>
-      <c r="B444" s="2" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A445" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="B445" s="2" t="s">
         <v>835</v>
-      </c>
-      <c r="B445" s="2" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A446" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B446" s="2" t="s">
         <v>837</v>
-      </c>
-      <c r="B446" s="2" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A447" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="B447" s="2" t="s">
         <v>839</v>
-      </c>
-      <c r="B447" s="2" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A448" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="B448" s="2" t="s">
         <v>841</v>
-      </c>
-      <c r="B448" s="2" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A449" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="B449" s="2" t="s">
         <v>843</v>
-      </c>
-      <c r="B449" s="2" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A450" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="B450" s="2" t="s">
         <v>845</v>
-      </c>
-      <c r="B450" s="2" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A451" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="B451" s="2" t="s">
         <v>847</v>
-      </c>
-      <c r="B451" s="2" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A452" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="B452" s="2" t="s">
         <v>849</v>
-      </c>
-      <c r="B452" s="2" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A453" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="B453" s="2" t="s">
         <v>851</v>
-      </c>
-      <c r="B453" s="2" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A454" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="B454" s="2" t="s">
         <v>853</v>
-      </c>
-      <c r="B454" s="2" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A455" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="B455" s="2" t="s">
         <v>855</v>
-      </c>
-      <c r="B455" s="2" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A456" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="B456" s="2" t="s">
         <v>857</v>
-      </c>
-      <c r="B456" s="2" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A457" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="B457" s="2" t="s">
         <v>859</v>
-      </c>
-      <c r="B457" s="2" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A458" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B458" s="2" t="s">
         <v>861</v>
-      </c>
-      <c r="B458" s="2" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A459" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="B459" s="2" t="s">
         <v>863</v>
-      </c>
-      <c r="B459" s="2" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A460" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="B460" s="2" t="s">
         <v>865</v>
-      </c>
-      <c r="B460" s="2" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A461" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B461" s="2" t="s">
         <v>867</v>
-      </c>
-      <c r="B461" s="2" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A462" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="B462" s="2" t="s">
         <v>869</v>
-      </c>
-      <c r="B462" s="2" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A463" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="B463" s="2" t="s">
         <v>871</v>
-      </c>
-      <c r="B463" s="2" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A464" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="B464" s="2" t="s">
         <v>873</v>
-      </c>
-      <c r="B464" s="2" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A465" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="B465" s="2" t="s">
         <v>875</v>
-      </c>
-      <c r="B465" s="2" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A466" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B466" s="2" t="s">
         <v>877</v>
-      </c>
-      <c r="B466" s="2" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A467" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B467" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A468" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B468" s="2" t="s">
         <v>880</v>
-      </c>
-      <c r="B468" s="2" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A469" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B469" s="2" t="s">
         <v>882</v>
-      </c>
-      <c r="B469" s="2" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A470" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B470" s="2" t="s">
         <v>884</v>
-      </c>
-      <c r="B470" s="2" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A471" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B471" s="2" t="s">
         <v>165</v>
@@ -7408,631 +7409,631 @@
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A472" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="B472" s="2" t="s">
         <v>887</v>
-      </c>
-      <c r="B472" s="2" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A473" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B473" s="2" t="s">
         <v>889</v>
-      </c>
-      <c r="B473" s="2" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A474" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="B474" s="2" t="s">
         <v>891</v>
-      </c>
-      <c r="B474" s="2" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A475" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="B475" s="2" t="s">
         <v>893</v>
-      </c>
-      <c r="B475" s="2" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A476" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="B476" s="2" t="s">
         <v>895</v>
-      </c>
-      <c r="B476" s="2" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A477" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="B477" s="2" t="s">
         <v>897</v>
-      </c>
-      <c r="B477" s="2" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A478" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B478" s="2" t="s">
         <v>899</v>
-      </c>
-      <c r="B478" s="2" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A479" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B479" s="2" t="s">
         <v>901</v>
-      </c>
-      <c r="B479" s="2" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A480" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="B480" s="2" t="s">
         <v>903</v>
-      </c>
-      <c r="B480" s="2" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A481" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B481" s="2" t="s">
         <v>905</v>
-      </c>
-      <c r="B481" s="2" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A482" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B482" s="2" t="s">
         <v>907</v>
-      </c>
-      <c r="B482" s="2" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A483" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="B483" s="2" t="s">
         <v>909</v>
-      </c>
-      <c r="B483" s="2" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A484" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="B484" s="2" t="s">
         <v>911</v>
-      </c>
-      <c r="B484" s="2" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A485" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="B485" s="2" t="s">
         <v>913</v>
-      </c>
-      <c r="B485" s="2" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A486" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B486" s="2" t="s">
         <v>915</v>
-      </c>
-      <c r="B486" s="2" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A487" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B487" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="488" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A488" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="B488" s="2" t="s">
         <v>918</v>
-      </c>
-      <c r="B488" s="2" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A489" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B489" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A490" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B490" s="2" t="s">
         <v>921</v>
-      </c>
-      <c r="B490" s="2" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A491" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B491" s="2" t="s">
         <v>923</v>
-      </c>
-      <c r="B491" s="2" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A492" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="B492" s="2" t="s">
         <v>925</v>
-      </c>
-      <c r="B492" s="2" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A493" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="B493" s="2" t="s">
         <v>927</v>
-      </c>
-      <c r="B493" s="2" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="494" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A494" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="B494" s="2" t="s">
         <v>929</v>
-      </c>
-      <c r="B494" s="2" t="s">
-        <v>930</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A495" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="B495" s="2" t="s">
         <v>931</v>
-      </c>
-      <c r="B495" s="2" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A496" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B496" s="2" t="s">
         <v>933</v>
-      </c>
-      <c r="B496" s="2" t="s">
-        <v>934</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A497" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="B497" s="2" t="s">
         <v>935</v>
-      </c>
-      <c r="B497" s="2" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A498" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="B498" s="2" t="s">
         <v>937</v>
-      </c>
-      <c r="B498" s="2" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A499" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="B499" s="2" t="s">
         <v>939</v>
-      </c>
-      <c r="B499" s="2" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A500" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="B500" s="2" t="s">
         <v>941</v>
-      </c>
-      <c r="B500" s="2" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A501" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="B501" s="2" t="s">
         <v>943</v>
-      </c>
-      <c r="B501" s="2" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A502" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="B502" s="2" t="s">
         <v>945</v>
-      </c>
-      <c r="B502" s="2" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A503" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="B503" s="2" t="s">
         <v>947</v>
-      </c>
-      <c r="B503" s="2" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A504" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="B504" s="2" t="s">
         <v>949</v>
-      </c>
-      <c r="B504" s="2" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A505" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="B505" s="2" t="s">
         <v>951</v>
-      </c>
-      <c r="B505" s="2" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A506" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="B506" s="2" t="s">
         <v>953</v>
-      </c>
-      <c r="B506" s="2" t="s">
-        <v>954</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A507" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="B507" s="2" t="s">
         <v>955</v>
-      </c>
-      <c r="B507" s="2" t="s">
-        <v>956</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A508" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B508" s="2" t="s">
         <v>957</v>
-      </c>
-      <c r="B508" s="2" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A509" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="B509" s="2" t="s">
         <v>959</v>
-      </c>
-      <c r="B509" s="2" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A510" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="B510" s="2" t="s">
         <v>961</v>
-      </c>
-      <c r="B510" s="2" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A511" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="B511" s="2" t="s">
         <v>963</v>
-      </c>
-      <c r="B511" s="2" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A512" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="B512" s="2" t="s">
         <v>965</v>
-      </c>
-      <c r="B512" s="2" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A513" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="B513" s="2" t="s">
         <v>967</v>
-      </c>
-      <c r="B513" s="2" t="s">
-        <v>968</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A514" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="B514" s="2" t="s">
         <v>969</v>
-      </c>
-      <c r="B514" s="2" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A515" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="B515" s="2" t="s">
         <v>971</v>
-      </c>
-      <c r="B515" s="2" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A516" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="B516" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="B516" s="2" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A517" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="B517" s="2" t="s">
         <v>975</v>
-      </c>
-      <c r="B517" s="2" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A518" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="B518" s="2" t="s">
         <v>977</v>
-      </c>
-      <c r="B518" s="2" t="s">
-        <v>978</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A519" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="B519" s="2" t="s">
         <v>979</v>
-      </c>
-      <c r="B519" s="2" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A520" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="B520" s="2" t="s">
         <v>981</v>
-      </c>
-      <c r="B520" s="2" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A521" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="B521" s="2" t="s">
         <v>983</v>
-      </c>
-      <c r="B521" s="2" t="s">
-        <v>984</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A522" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="B522" s="2" t="s">
         <v>985</v>
-      </c>
-      <c r="B522" s="2" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A523" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="B523" s="2" t="s">
         <v>987</v>
-      </c>
-      <c r="B523" s="2" t="s">
-        <v>988</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A524" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="B524" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="B524" s="2" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A525" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="B525" s="2" t="s">
         <v>991</v>
-      </c>
-      <c r="B525" s="2" t="s">
-        <v>992</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A526" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="B526" s="2" t="s">
         <v>993</v>
-      </c>
-      <c r="B526" s="2" t="s">
-        <v>994</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A527" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="B527" s="2" t="s">
         <v>995</v>
-      </c>
-      <c r="B527" s="2" t="s">
-        <v>996</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A528" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="B528" s="2" t="s">
         <v>997</v>
-      </c>
-      <c r="B528" s="2" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A529" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="B529" s="2" t="s">
         <v>999</v>
-      </c>
-      <c r="B529" s="2" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A530" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B530" s="2" t="s">
         <v>1001</v>
-      </c>
-      <c r="B530" s="2" t="s">
-        <v>1002</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A531" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B531" s="2" t="s">
         <v>1003</v>
-      </c>
-      <c r="B531" s="2" t="s">
-        <v>1004</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A532" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B532" s="2" t="s">
         <v>1005</v>
-      </c>
-      <c r="B532" s="2" t="s">
-        <v>1006</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A533" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B533" s="2" t="s">
         <v>1007</v>
-      </c>
-      <c r="B533" s="2" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A534" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B534" s="2" t="s">
         <v>1009</v>
-      </c>
-      <c r="B534" s="2" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A535" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B535" s="2" t="s">
         <v>1011</v>
-      </c>
-      <c r="B535" s="2" t="s">
-        <v>1012</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A536" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B536" s="2" t="s">
         <v>1013</v>
-      </c>
-      <c r="B536" s="2" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A537" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B537" s="2" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A538" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B538" s="2" t="s">
         <v>1016</v>
-      </c>
-      <c r="B538" s="2" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A539" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B539" s="2" t="s">
         <v>1018</v>
-      </c>
-      <c r="B539" s="2" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A540" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B540" s="2" t="s">
         <v>1020</v>
-      </c>
-      <c r="B540" s="2" t="s">
-        <v>1021</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A541" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B541" s="2" t="s">
         <v>1022</v>
-      </c>
-      <c r="B541" s="2" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A542" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B542" s="2" t="s">
         <v>1024</v>
-      </c>
-      <c r="B542" s="2" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A543" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B543" s="2" t="s">
         <v>1026</v>
-      </c>
-      <c r="B543" s="2" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A544" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B544" s="2" t="s">
         <v>1028</v>
-      </c>
-      <c r="B544" s="2" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A545" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B545" s="2" t="s">
         <v>1030</v>
-      </c>
-      <c r="B545" s="2" t="s">
-        <v>1031</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A546" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B546" s="2" t="s">
         <v>1032</v>
-      </c>
-      <c r="B546" s="2" t="s">
-        <v>1033</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A547" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B547" s="2" t="s">
         <v>1034</v>
-      </c>
-      <c r="B547" s="2" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A548" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B548" s="2" t="s">
         <v>1036</v>
-      </c>
-      <c r="B548" s="2" t="s">
-        <v>1037</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A549" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B549" s="2" t="s">
         <v>1038</v>
-      </c>
-      <c r="B549" s="2" t="s">
-        <v>1039</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A550" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B550" s="2" t="s">
         <v>49</v>
@@ -8040,103 +8041,103 @@
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A551" s="4" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B551" s="3" t="s">
         <v>1043</v>
-      </c>
-      <c r="B551" s="3" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A552" s="4" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B552" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A553" s="4" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B553" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="554" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A554" s="4" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B554" s="3" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="555" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A555" s="4" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B555" s="3" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A556" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A557" s="4" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B557" s="3" t="s">
         <v>1053</v>
-      </c>
-      <c r="B557" s="3" t="s">
-        <v>1054</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A558" s="4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B558" s="3" t="s">
         <v>1055</v>
-      </c>
-      <c r="B558" s="3" t="s">
-        <v>1056</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A559" s="4" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B559" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A560" s="4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B560" s="3" t="s">
         <v>1058</v>
-      </c>
-      <c r="B560" s="3" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A561" s="4" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B561" s="3" t="s">
         <v>1061</v>
-      </c>
-      <c r="B561" s="3" t="s">
-        <v>1062</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A562" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B562" s="3" t="s">
         <v>1065</v>
-      </c>
-      <c r="B562" s="3" t="s">
-        <v>1066</v>
       </c>
     </row>
     <row r="563" spans="1:2" ht="52.5" x14ac:dyDescent="0.3">
       <c r="A563" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B563" s="3" t="s">
         <v>1067</v>
-      </c>
-      <c r="B563" s="3" t="s">
-        <v>1068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more Lua functions
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCC112B-D7B9-4106-8F51-0D9862E153D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E1EBFB-70E2-44FC-A95C-F4554D8FFB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="2120" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="1091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="1093">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3354,6 +3354,14 @@
   </si>
   <si>
     <t>移动节点</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LuaConsole.InputBoxTitle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>请输入</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3730,10 +3738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B574"/>
+  <dimension ref="A1:B575"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A555" workbookViewId="0">
-      <selection activeCell="B560" sqref="B560"/>
+      <selection activeCell="B569" sqref="B569:B570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8310,9 +8318,17 @@
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A574" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B574" s="3" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A575" s="4" t="s">
         <v>1089</v>
       </c>
-      <c r="B574" s="3" t="s">
+      <c r="B575" s="3" t="s">
         <v>1090</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add map annotation function
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E1EBFB-70E2-44FC-A95C-F4554D8FFB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897BD610-755E-4372-8284-193E57AB2E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="2120" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="1093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="1109">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3362,6 +3362,66 @@
   </si>
   <si>
     <t>请输入</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入注释</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除注释</t>
+  </si>
+  <si>
+    <t>AnnotationObListDelete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnnotationCaption</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>字体大小：</t>
+  </si>
+  <si>
+    <t>文本颜色：</t>
+  </si>
+  <si>
+    <t>背景颜色：</t>
+  </si>
+  <si>
+    <t>AnnotationBackgroundColor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnnotationTextColor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnnotationFontSize</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnnotationBold</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>粗体</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnnotationObList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图注释</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnnotationObListAddChange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增/修改注释</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3738,10 +3798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B575"/>
+  <dimension ref="A1:B583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A555" workbookViewId="0">
-      <selection activeCell="B569" sqref="B569:B570"/>
+    <sheetView tabSelected="1" topLeftCell="A563" workbookViewId="0">
+      <selection activeCell="B578" sqref="B578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8332,6 +8392,70 @@
         <v>1090</v>
       </c>
     </row>
+    <row r="576" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A576" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B576" s="3" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A577" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B577" s="3" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A578" s="4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B578" s="3" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A579" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B579" s="3" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="580" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A580" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B580" s="3" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="581" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A581" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B581" s="3" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A582" s="4" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B582" s="3" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A583" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B583" s="3" t="s">
+        <v>1106</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
restore "add trigger in this group" function
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897BD610-755E-4372-8284-193E57AB2E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F98845-9D3D-4B41-A642-20C6A306D3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="2120" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10160" yWindow="140" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="1119">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3422,6 +3422,41 @@
   </si>
   <si>
     <t>新增/修改注释</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>在本组新建触发</t>
+  </si>
+  <si>
+    <t>在本组新建标签</t>
+  </si>
+  <si>
+    <t>在本组新建脚本</t>
+  </si>
+  <si>
+    <t>在本组新建作战小队</t>
+  </si>
+  <si>
+    <t>在本组新建特遣部队</t>
+  </si>
+  <si>
+    <t>TaskForceSortNewTaskForce</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TeamSortNewTeam</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScriptSortNewScript</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TagSortNewTag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TriggerSortNewTrigger</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3798,10 +3833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B583"/>
+  <dimension ref="A1:B588"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A563" workbookViewId="0">
-      <selection activeCell="B578" sqref="B578"/>
+    <sheetView tabSelected="1" topLeftCell="A562" workbookViewId="0">
+      <selection activeCell="B579" sqref="B579"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8456,6 +8491,46 @@
         <v>1106</v>
       </c>
     </row>
+    <row r="584" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A584" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B584" s="3" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="585" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A585" s="4" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B585" s="3" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="586" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A586" s="4" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B586" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="587" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A587" s="4" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B587" s="3" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="588" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A588" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B588" s="3" t="s">
+        <v>1113</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support multi-select same connected tiles
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F98845-9D3D-4B41-A642-20C6A306D3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C12D2DC-F311-4774-91E5-0CE4FA338EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10160" yWindow="140" windowWidth="28230" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="720" windowWidth="28210" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="1119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="1123">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3457,6 +3457,20 @@
   </si>
   <si>
     <t>TriggerSortNewTrigger</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>同类相连添加</t>
+  </si>
+  <si>
+    <t>同类相连删除</t>
+  </si>
+  <si>
+    <t>MultiSelectionConnectedDelete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultiSelectionConnectedAdd</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3833,10 +3847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B588"/>
+  <dimension ref="A1:B590"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A562" workbookViewId="0">
-      <selection activeCell="B579" sqref="B579"/>
+    <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
+      <selection activeCell="B585" sqref="B585"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8531,6 +8545,22 @@
         <v>1113</v>
       </c>
     </row>
+    <row r="589" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A589" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B589" s="3" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="590" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A590" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B590" s="3" t="s">
+        <v>1120</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
multi-select now consider lat; improve lat efficiency
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C12D2DC-F311-4774-91E5-0CE4FA338EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A15C79-89DB-45B2-A058-6694F0C1C716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="720" windowWidth="28210" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="380" windowWidth="28210" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="1125">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3472,6 +3472,13 @@
   <si>
     <t>MultiSelectionConnectedAdd</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultiSelectionHide</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏多选单元格</t>
   </si>
 </sst>
 </file>
@@ -3847,10 +3854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B590"/>
+  <dimension ref="A1:B591"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
-      <selection activeCell="B585" sqref="B585"/>
+      <selection activeCell="G577" sqref="G577"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8561,6 +8568,14 @@
         <v>1120</v>
       </c>
     </row>
+    <row r="591" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A591" s="4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B591" s="3" t="s">
+        <v>1124</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add paste show outline menu
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A15C79-89DB-45B2-A058-6694F0C1C716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDFAA9B-63E1-4668-A141-B53272216D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="380" windowWidth="28210" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="1127">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3479,6 +3479,14 @@
   </si>
   <si>
     <t>隐藏多选单元格</t>
+  </si>
+  <si>
+    <t>粘贴区域描边</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.Paste.ShowOutline</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3854,10 +3862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B591"/>
+  <dimension ref="A1:B592"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
-      <selection activeCell="G577" sqref="G577"/>
+      <selection activeCell="B589" sqref="B589"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8576,6 +8584,14 @@
         <v>1124</v>
       </c>
     </row>
+    <row r="592" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A592" s="4" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B592" s="3" t="s">
+        <v>1125</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add toggle button, add cameo for root nodes
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDFAA9B-63E1-4668-A141-B53272216D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582303A7-15B4-40EB-978F-8C3FE6FF1356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="380" windowWidth="28210" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="1129">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3486,6 +3486,14 @@
   </si>
   <si>
     <t>Menu.Paste.ShowOutline</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.Options.ShowObjectViewCameo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示物品浏览器图标</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3862,7 +3870,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B592"/>
+  <dimension ref="A1:B593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
       <selection activeCell="B589" sqref="B589"/>
@@ -8592,6 +8600,14 @@
         <v>1125</v>
       </c>
     </row>
+    <row r="593" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A593" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B593" s="3" t="s">
+        <v>1128</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rewrite tunnel tool, update cameos
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582303A7-15B4-40EB-978F-8C3FE6FF1356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3459A869-C8AD-4E53-9A1A-9ED8A980CF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="380" windowWidth="28210" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="1139">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3495,6 +3495,41 @@
   <si>
     <t>显示物品浏览器图标</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ErrorTooLongTube</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不能创建过长的隧道！</t>
+  </si>
+  <si>
+    <t>NewUnidirectionalTunnelObList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>建立单向隧道</t>
+  </si>
+  <si>
+    <t>MV_ValidateTubeTooLong</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>隧道 - %1 长度超过100！请检查。</t>
+  </si>
+  <si>
+    <t>MV_ValidateTubeUnidirection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>隧道 - %1 是单向的！请检查。</t>
+  </si>
+  <si>
+    <t>MV_ValidateTubeMultiShare</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>多个隧道在 %1 端点重叠。请检查。</t>
   </si>
 </sst>
 </file>
@@ -3870,7 +3905,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B593"/>
+  <dimension ref="A1:B598"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
       <selection activeCell="B589" sqref="B589"/>
@@ -8608,6 +8643,46 @@
         <v>1128</v>
       </c>
     </row>
+    <row r="594" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A594" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B594" s="3" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A595" s="4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B595" s="3" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A596" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B596" s="3" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A597" s="4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B597" s="3" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A598" s="4" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B598" s="3" t="s">
+        <v>1138</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
improve scaling efficiency, add multi select options
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3459A869-C8AD-4E53-9A1A-9ED8A980CF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA00417-BD09-432D-B110-C26F14C19724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="380" windowWidth="28210" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="1155">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3530,6 +3530,56 @@
   </si>
   <si>
     <t>多个隧道在 %1 端点重叠。请检查。</t>
+  </si>
+  <si>
+    <t>MultiSelectionOptionCaption</t>
+  </si>
+  <si>
+    <t>多选选项</t>
+  </si>
+  <si>
+    <t>MultiSelectionOptionConnected</t>
+  </si>
+  <si>
+    <t>相连</t>
+  </si>
+  <si>
+    <t>MultiSelectionOptionSameTileSet</t>
+  </si>
+  <si>
+    <t>相同地形组</t>
+  </si>
+  <si>
+    <t>MultiSelectionOptionConsiderLAT</t>
+  </si>
+  <si>
+    <t>考虑LAT</t>
+  </si>
+  <si>
+    <t>MultiSelectionOptionSameHeight</t>
+  </si>
+  <si>
+    <t>相同高度</t>
+  </si>
+  <si>
+    <t>MultiSelectionOptionSameBaiscHeight</t>
+  </si>
+  <si>
+    <t>相同基础高度</t>
+  </si>
+  <si>
+    <t>自定义添加</t>
+  </si>
+  <si>
+    <t>自定义删除</t>
+  </si>
+  <si>
+    <t>MultiSelectionCustomDelete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultiSelectionCustomAdd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3905,10 +3955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B598"/>
+  <dimension ref="A1:B606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
-      <selection activeCell="B589" sqref="B589"/>
+    <sheetView tabSelected="1" topLeftCell="A579" workbookViewId="0">
+      <selection activeCell="A601" sqref="A601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8683,6 +8733,70 @@
         <v>1138</v>
       </c>
     </row>
+    <row r="599" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A599" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B599" s="3" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A600" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B600" s="3" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A601" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B601" s="3" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A602" s="4" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B602" s="3" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A603" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B603" s="3" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A604" s="4" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B604" s="3" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A605" s="4" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B605" s="3" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A606" s="4" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B606" s="3" t="s">
+        <v>1152</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add Lua brush and demo scripts
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA00417-BD09-432D-B110-C26F14C19724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56DD0CB-DB23-4C86-B46F-2C22D5F9F109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="380" windowWidth="28210" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6630" yWindow="3980" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="1155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="1157">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3289,10 +3289,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>点击“运行脚本”以执行所选的Lua脚本，点击“执行输入”以执行输入窗口中的代码。脚本可能会损坏地图，请在运行前保存或执行快照函数。请参阅文档了解可用函数。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>LuaScriptConsoleInput</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3317,22 +3313,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>LuaScriptConsoleExecute</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>运行脚本</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>LuaScriptConsoleRun</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>执行输入</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>LuaConsole.SnapshotConfirmTitle</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3579,6 +3563,27 @@
   </si>
   <si>
     <t>MultiSelectionCustomAdd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>勾选“执行文件”以读取选中的Lua脚本，否则读取输入窗口。点击“执行”以执行所选的代码。点击“脚本刷”在地图的指定坐标执行脚本。脚本可能会损坏地图，请在运行前保存或执行快照函数。请参阅文档了解可用函数。</t>
+  </si>
+  <si>
+    <t>脚本刷</t>
+  </si>
+  <si>
+    <t>LuaScriptConsoleRunFile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>执行文件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>执行</t>
+  </si>
+  <si>
+    <t>LuaScriptConsoleBrush</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3955,10 +3960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B606"/>
+  <dimension ref="A1:B607"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A579" workbookViewId="0">
-      <selection activeCell="A601" sqref="A601"/>
+    <sheetView tabSelected="1" topLeftCell="A593" workbookViewId="0">
+      <selection activeCell="B602" sqref="B602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8469,52 +8474,52 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="566" spans="1:2" ht="52.5" x14ac:dyDescent="0.3">
+    <row r="566" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A566" s="4" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B566" s="3" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A567" s="4" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B567" s="3" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A568" s="4" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B568" s="3" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A569" s="4" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="B569" s="3" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A570" s="4" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="B570" s="3" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A571" s="4" t="s">
-        <v>1083</v>
+        <v>1087</v>
       </c>
       <c r="B571" s="3" t="s">
-        <v>1084</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.3">
@@ -8527,26 +8532,26 @@
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A573" s="4" t="s">
-        <v>1087</v>
+        <v>1092</v>
       </c>
       <c r="B573" s="3" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A574" s="4" t="s">
-        <v>1091</v>
+        <v>1098</v>
       </c>
       <c r="B574" s="3" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A575" s="4" t="s">
-        <v>1089</v>
+        <v>1097</v>
       </c>
       <c r="B575" s="3" t="s">
-        <v>1090</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.3">
@@ -8554,103 +8559,103 @@
         <v>1096</v>
       </c>
       <c r="B576" s="3" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A577" s="4" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="B577" s="3" t="s">
-        <v>1097</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A578" s="4" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="B578" s="3" t="s">
-        <v>1098</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A579" s="4" t="s">
-        <v>1100</v>
+        <v>1091</v>
       </c>
       <c r="B579" s="3" t="s">
-        <v>1099</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A580" s="4" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="B580" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A581" s="4" t="s">
-        <v>1107</v>
+        <v>1114</v>
       </c>
       <c r="B581" s="3" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A582" s="4" t="s">
-        <v>1095</v>
+        <v>1113</v>
       </c>
       <c r="B582" s="3" t="s">
-        <v>1094</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A583" s="4" t="s">
-        <v>1105</v>
+        <v>1112</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A584" s="4" t="s">
-        <v>1118</v>
+        <v>1111</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A585" s="4" t="s">
-        <v>1117</v>
+        <v>1110</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A586" s="4" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="B586" s="3" t="s">
-        <v>1111</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A587" s="4" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="B587" s="3" t="s">
-        <v>1112</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A588" s="4" t="s">
-        <v>1114</v>
+        <v>1119</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1113</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.3">
@@ -8658,116 +8663,116 @@
         <v>1122</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A590" s="4" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1120</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A591" s="4" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="B591" s="3" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A592" s="4" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="B592" s="3" t="s">
-        <v>1125</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A593" s="4" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="B593" s="3" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A594" s="4" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="B594" s="3" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A595" s="4" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="B595" s="3" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A596" s="4" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="B596" s="3" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A597" s="4" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="B597" s="3" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A598" s="4" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="B598" s="3" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A599" s="4" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="B599" s="3" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A600" s="4" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="B600" s="3" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A601" s="4" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="B601" s="3" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A602" s="4" t="s">
-        <v>1145</v>
+        <v>1150</v>
       </c>
       <c r="B602" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A603" s="4" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="B603" s="3" t="s">
         <v>1148</v>
@@ -8775,26 +8780,34 @@
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A604" s="4" t="s">
-        <v>1149</v>
+        <v>1080</v>
       </c>
       <c r="B604" s="3" t="s">
-        <v>1150</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A605" s="4" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B605" s="3" t="s">
         <v>1154</v>
-      </c>
-      <c r="B605" s="3" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A606" s="4" t="s">
-        <v>1153</v>
+        <v>1156</v>
       </c>
       <c r="B606" s="3" t="s">
         <v>1152</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" ht="70" x14ac:dyDescent="0.3">
+      <c r="A607" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B607" s="3" t="s">
+        <v>1151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rewrite local variable & support search ref
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56DD0CB-DB23-4C86-B46F-2C22D5F9F109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B12581E-9888-45B7-9315-33CB9F138CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6630" yWindow="3980" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="1168">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3584,6 +3584,45 @@
   </si>
   <si>
     <t>LuaScriptConsoleBrush</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>局部变量</t>
+  </si>
+  <si>
+    <t>选择局部变量：</t>
+  </si>
+  <si>
+    <t>名称：</t>
+  </si>
+  <si>
+    <t>初始值：</t>
+  </si>
+  <si>
+    <t>LocalVariablesNew</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalVariablesValue</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalVariablesName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalVariablesSelect</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalVariablesTitle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SearchReferenceScriptLine</t>
+  </si>
+  <si>
+    <t>脚本行</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3960,10 +3999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B607"/>
+  <dimension ref="A1:B613"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A593" workbookViewId="0">
-      <selection activeCell="B602" sqref="B602"/>
+      <selection activeCell="B613" sqref="B613"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8810,6 +8849,54 @@
         <v>1151</v>
       </c>
     </row>
+    <row r="608" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A608" s="4" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B608" s="3" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A609" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B609" s="3" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A610" s="4" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B610" s="3" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A611" s="4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B611" s="3" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A612" s="4" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B612" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A613" s="4" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B613" s="3" t="s">
+        <v>1167</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rewrite drawmap(), add building foundation classification
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B12581E-9888-45B7-9315-33CB9F138CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC8FCAC-2C37-432D-9A44-4CF18CD18306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6630" yWindow="3980" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="1170">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3623,6 +3623,13 @@
   </si>
   <si>
     <t>脚本行</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FoundationBuildingObList</t>
+  </si>
+  <si>
+    <t>建筑</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3999,10 +4006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B613"/>
+  <dimension ref="A1:B614"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A593" workbookViewId="0">
-      <selection activeCell="B613" sqref="B613"/>
+      <selection activeCell="B612" sqref="B612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8897,6 +8904,14 @@
         <v>1167</v>
       </c>
     </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A614" s="4" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B614" s="3" t="s">
+        <v>1169</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change image sever to x86, add terrain into server
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC8FCAC-2C37-432D-9A44-4CF18CD18306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CFFA93-DD6D-4482-AEF6-B901AD473AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6630" yWindow="3980" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9960" yWindow="3980" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="1172">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3630,6 +3630,14 @@
   </si>
   <si>
     <t>建筑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LaunchImageServerFailed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>无法启动图像服务器！\n请检查ImageServer.exe是否存在，\n或关闭LoadImageDataFromServer。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4006,10 +4014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B614"/>
+  <dimension ref="A1:B615"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A593" workbookViewId="0">
-      <selection activeCell="B612" sqref="B612"/>
+      <selection activeCell="D611" sqref="D611"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8912,6 +8920,14 @@
         <v>1169</v>
       </c>
     </row>
+    <row r="615" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+      <c r="A615" s="4" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B615" s="3" t="s">
+        <v>1171</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support phobos actioon 606-608
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CFFA93-DD6D-4482-AEF6-B901AD473AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704DA080-0E07-4303-81AD-7D33A1C8858F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="3980" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="1172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="1174">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3639,6 +3639,13 @@
   <si>
     <t>无法启动图像服务器！\n请检查ImageServer.exe是否存在，\n或关闭LoadImageDataFromServer。</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Allhouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>全部所属方</t>
   </si>
 </sst>
 </file>
@@ -4014,10 +4021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B615"/>
+  <dimension ref="A1:B616"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A593" workbookViewId="0">
-      <selection activeCell="D611" sqref="D611"/>
+      <selection activeCell="B616" sqref="B616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8928,6 +8935,14 @@
         <v>1171</v>
       </c>
     </row>
+    <row r="616" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A616" s="4" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B616" s="3" t="s">
+        <v>1173</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
multi selection can display tile count
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704DA080-0E07-4303-81AD-7D33A1C8858F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9F27CA-6D24-4707-8449-4695DFCA2930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="3980" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2570" yWindow="3980" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="1174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="1180">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3646,6 +3646,29 @@
   </si>
   <si>
     <t>全部所属方</t>
+  </si>
+  <si>
+    <t>, 单元格数量: %d</t>
+  </si>
+  <si>
+    <t>MoneyOnMap.MultiSelectionCoords</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CancelForceEnemy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>强制没有敌人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>解除强制宣战</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ForceNoEnemy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4021,10 +4044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B616"/>
+  <dimension ref="A1:B619"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A593" workbookViewId="0">
-      <selection activeCell="B616" sqref="B616"/>
+    <sheetView tabSelected="1" topLeftCell="A602" workbookViewId="0">
+      <selection activeCell="B615" sqref="B615"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8943,6 +8966,30 @@
         <v>1173</v>
       </c>
     </row>
+    <row r="617" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A617" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B617" s="3" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A618" s="4" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B618" s="3" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A619" s="4" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B619" s="3" t="s">
+        <v>1174</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add preference dialog, all dialogs support F5 refresh
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9F27CA-6D24-4707-8449-4695DFCA2930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C69A96-3E77-4189-845A-5035BB0477A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2570" yWindow="3980" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9460" yWindow="3090" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="1334">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3668,6 +3668,548 @@
   </si>
   <si>
     <t>ForceNoEnemy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>局部变量的数量超过100，超出的变量将无法使用。如果你使用了Phobos，请开启ExtVariables。</t>
+  </si>
+  <si>
+    <t>局部变量过多</t>
+  </si>
+  <si>
+    <t>偏好设置</t>
+  </si>
+  <si>
+    <t>设置项</t>
+  </si>
+  <si>
+    <t>重新加载地图以应用此修改</t>
+  </si>
+  <si>
+    <t>重新启动FA2以应用此修改</t>
+  </si>
+  <si>
+    <t>屏蔽不可用所属方</t>
+  </si>
+  <si>
+    <t>将建筑按大小分类</t>
+  </si>
+  <si>
+    <t>在月球地图显示水面地形</t>
+  </si>
+  <si>
+    <t>加载平民建筑的额外翻译</t>
+  </si>
+  <si>
+    <t>从地图文件夹重新读取资源文件</t>
+  </si>
+  <si>
+    <t>读取#include INI (Ares)</t>
+  </si>
+  <si>
+    <t>编辑CSF触发参数时弹出CSF浏览器</t>
+  </si>
+  <si>
+    <t>复制触发/小队等时递增编号</t>
+  </si>
+  <si>
+    <t>自动调整下拉菜单宽度</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序触发/小队等</t>
+  </si>
+  <si>
+    <t>编辑路径点参数时弹出下拉菜单</t>
+  </si>
+  <si>
+    <t>根据高度显示不同鼠标颜色</t>
+  </si>
+  <si>
+    <t>自动保存地图</t>
+  </si>
+  <si>
+    <t>仅以.map格式保存地图</t>
+  </si>
+  <si>
+    <t>生成更精细的多人游戏预览图</t>
+  </si>
+  <si>
+    <t>地图开头添加编码警告的注释</t>
+  </si>
+  <si>
+    <t>启用无限路径点 (Phobos)</t>
+  </si>
+  <si>
+    <t>启用无限变量 (Phobos)</t>
+  </si>
+  <si>
+    <t>按住shift放置地形时仅记录一次历史</t>
+  </si>
+  <si>
+    <t>按住shift放置覆盖图时仅记录一次历史</t>
+  </si>
+  <si>
+    <t>为路径点绘制矩形背景</t>
+  </si>
+  <si>
+    <t>为基地节点索引绘制矩形背景</t>
+  </si>
+  <si>
+    <t>将地形浏览器移至右侧</t>
+  </si>
+  <si>
+    <t>启用新的视觉样式(可能无法输入中文)</t>
+  </si>
+  <si>
+    <t>在随机树木窗口显示所有地形对象</t>
+  </si>
+  <si>
+    <t>在显存中分配DirectDraw surface</t>
+  </si>
+  <si>
+    <t>在DirectDrawCreate中使用emulation mode</t>
+  </si>
+  <si>
+    <t>使用双线性插值缩放绘图界面(更精细，但更卡)</t>
+  </si>
+  <si>
+    <t>使用独立服务器进程存储游戏素材</t>
+  </si>
+  <si>
+    <t>不将所属方翻译为其UIName</t>
+  </si>
+  <si>
+    <t>翻译所属方的同时显示英文原名</t>
+  </si>
+  <si>
+    <t>地图检查器的新检查仅弹出提示而非错误</t>
+  </si>
+  <si>
+    <t>地图检查器的INI长度限制为512而非128 (Ares)</t>
+  </si>
+  <si>
+    <t>加载素材启用严格NewTheater逻辑</t>
+  </si>
+  <si>
+    <t>禁止摆放重叠建筑</t>
+  </si>
+  <si>
+    <t>自动填写Upgrade数量</t>
+  </si>
+  <si>
+    <t>建筑存在Upgrade时设为满血</t>
+  </si>
+  <si>
+    <t>使用默认光照时调整单位RGB值</t>
+  </si>
+  <si>
+    <t>在小地图显示可视地图边界</t>
+  </si>
+  <si>
+    <t>第一个步兵放置在最下方(4号subcell)</t>
+  </si>
+  <si>
+    <t>编辑步兵时考虑鼠标位置</t>
+  </si>
+  <si>
+    <t>单元格只有单步兵时仍判断鼠标位置</t>
+  </si>
+  <si>
+    <t>拖拽步兵时考虑鼠标位置</t>
+  </si>
+  <si>
+    <t>放置步兵时考虑鼠标位置</t>
+  </si>
+  <si>
+    <t>固定中间步兵位置同InfantrySubCell.GameDefault</t>
+  </si>
+  <si>
+    <t>放置步兵时考虑地形对象占用</t>
+  </si>
+  <si>
+    <t>强制CString内存在堆上分配</t>
+  </si>
+  <si>
+    <t>启用严格错误捕获(会捕获C++ EH错误)</t>
+  </si>
+  <si>
+    <t>使用新的工具栏图标</t>
+  </si>
+  <si>
+    <t>不显示今日提示窗口</t>
+  </si>
+  <si>
+    <t>选择地形工具时不改变笔刷大小</t>
+  </si>
+  <si>
+    <t>放置地形时跳过隐藏单元格</t>
+  </si>
+  <si>
+    <t>在INI编辑器中忽略小队/特遣/脚本小节</t>
+  </si>
+  <si>
+    <t>ctrl填充地形时同时填充LAT</t>
+  </si>
+  <si>
+    <t>ctrl填充地形时将水面视为一类</t>
+  </si>
+  <si>
+    <t>加载并显示阴影</t>
+  </si>
+  <si>
+    <t>加载并显示可部署单位的更换图像</t>
+  </si>
+  <si>
+    <t>加载并显示水中单位的更换图像</t>
+  </si>
+  <si>
+    <t>加载并显示单位伤残的更换图像 (Phobos)</t>
+  </si>
+  <si>
+    <t>将悬浮单位渲染的更高</t>
+  </si>
+  <si>
+    <t>显示建筑物和地形对象的AlphaImage</t>
+  </si>
+  <si>
+    <t>将桥梁上单位渲染的更高</t>
+  </si>
+  <si>
+    <t>开启平面显示时隐藏地形ExtraImage</t>
+  </si>
+  <si>
+    <t>显示地图边界外的游戏对象</t>
+  </si>
+  <si>
+    <t>单位选项窗口显示&lt;Player @ X&gt;所属方 (Phobos)</t>
+  </si>
+  <si>
+    <t>检测地图文件的外部修改</t>
+  </si>
+  <si>
+    <t>计算武器射程时考虑悬崖影响</t>
+  </si>
+  <si>
+    <t>粘贴地形时默认显示描边</t>
+  </si>
+  <si>
+    <t>LocalVariablesExceed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalVariablesExceedTitle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.Options.Preferences</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.Label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ReloadMap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.Restart</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ObjectBrowser.SafeHouses</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ObjectBrowser.Foundation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.LoadLunarWater</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.LoadCivilianStringtable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ReloadGameFromMapFolder</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.AllowIncludes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.AllowPlusEqual</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ArtImageSwap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.TutorialTexts.Viewer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.CloneWithOrderedID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.AdjustDropdownWidth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SortByLabelName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SearchCombobox.Waypoint</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.CursorSelectionBound.AutoHeightColor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SaveMap.AutoSave</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SaveMap.OnlySaveMAP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SaveMap.BetterMapPreview</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SaveMap.FileEncodingComment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtWaypoints</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtVariables</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.UndoRedo.ShiftPlaceTile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.UndoRedo.HoldPlaceOverlay</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.Waypoint.Background</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.BaseNodeIndex.Background</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.VerticalLayout</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.EnableVisualStyle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.RandomTerrainObjects</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.DDrawInVideoMem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.DDrawEmulation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.DDrawScalingBilinear</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.LoadImageDataFromServer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.NoHouseNameTranslation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.BetterHouseNameTranslation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtendedValidationNoError</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtendedValidationAres</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.HideNoRubbleBuilding</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.UseStrictNewTheater</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PlaceStructure.OverlappingCheck</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PlaceStructure.AutoUpgrade</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PlaceStructure.UpgradeStrength</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.LightingPreview.MultUnitColor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ShowMapBoundInMiniMap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.GameDefault</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.Edit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.Edit.Single</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.Edit.Drag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.Edit.Place</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.Edit.FixCenter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.OccupationBits</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.StringBufferStackAllocation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.StrictExceptionFilter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.UseNewToolBarCameo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SkipTipsOfTheDay</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SkipBrushSizeChangeOnTools</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PlaceTileSkipHide</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.INIEditor.IgnoreTeams</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.FillArea.ConsiderLAT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.FillArea.ConsiderWater</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Shadow</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Deploy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Water</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Damage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Hover</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.AlphaImage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Bridge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.FlatToGroundHideExtra</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.DisplayObjectsOutside</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PlayerAtXForTechnos</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.FileWatcher</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.WeaponRangeBound.SubjectToElevation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PasteShowOutline</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不渲染HP=0且LeaveRubble=no的建筑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取注册表小节的+= (Ares)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取单位art(md).ini中的Image= (Phobos)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3675,7 +4217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3714,6 +4256,14 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3747,7 +4297,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3762,6 +4312,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4044,10 +4597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B619"/>
+  <dimension ref="A1:D696"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A602" workbookViewId="0">
-      <selection activeCell="B615" sqref="B615"/>
+    <sheetView tabSelected="1" topLeftCell="A672" workbookViewId="0">
+      <selection activeCell="B631" sqref="B631"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -8990,6 +9543,626 @@
         <v>1174</v>
       </c>
     </row>
+    <row r="620" spans="1:2" ht="35" x14ac:dyDescent="0.3">
+      <c r="A620" s="4" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B620" s="3" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A621" s="4" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B621" s="3" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="622" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A622" s="4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B622" s="3" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="623" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A623" s="4" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B623" s="3" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="624" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A624" s="4" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B624" s="3" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A625" s="4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B625" s="3" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A626" s="4" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B626" s="3" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A627" s="4" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B627" s="3" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="628" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A628" s="4" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B628" s="3" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A629" s="4" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B629" s="3" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A630" s="4" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B630" s="3" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="631" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A631" s="4" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B631" s="3" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="632" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A632" s="4" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B632" s="3" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C632" s="7"/>
+    </row>
+    <row r="633" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A633" s="4" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B633" s="3" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C633" s="7"/>
+    </row>
+    <row r="634" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A634" s="4" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B634" s="3" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="635" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A635" s="4" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B635" s="3" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="636" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A636" s="4" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B636" s="3" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="637" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A637" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B637" s="3" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="638" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A638" s="4" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B638" s="3" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="639" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A639" s="4" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B639" s="3" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="640" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A640" s="4" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B640" s="3" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A641" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B641" s="3" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="642" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A642" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B642" s="3" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="643" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A643" s="4" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B643" s="3" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="644" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A644" s="4" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B644" s="3" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="645" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A645" s="4" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B645" s="3" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="646" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A646" s="4" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B646" s="3" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A647" s="4" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B647" s="3" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="648" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A648" s="4" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B648" s="3" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A649" s="4" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B649" s="3" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="650" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A650" s="4" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B650" s="3" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="651" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A651" s="4" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B651" s="3" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="652" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A652" s="4" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B652" s="3" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A653" s="4" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B653" s="3" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A654" s="4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B654" s="3" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A655" s="4" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B655" s="3" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A656" s="4" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B656" s="3" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="657" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A657" s="4" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B657" s="3" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="658" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A658" s="4" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B658" s="3" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="659" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A659" s="4" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B659" s="3" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="660" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A660" s="4" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B660" s="3" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="661" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A661" s="4" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B661" s="3" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C661" s="7"/>
+      <c r="D661" s="7"/>
+    </row>
+    <row r="662" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A662" s="4" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B662" s="3" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="663" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A663" s="4" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B663" s="3" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="664" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A664" s="4" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B664" s="3" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="665" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A665" s="4" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B665" s="3" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="666" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A666" s="4" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B666" s="3" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="667" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A667" s="4" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B667" s="3" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="668" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A668" s="4" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B668" s="3" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="669" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A669" s="4" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B669" s="3" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="670" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A670" s="4" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B670" s="3" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="671" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A671" s="4" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B671" s="3" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="672" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A672" s="4" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B672" s="3" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A673" s="4" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B673" s="3" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A674" s="4" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B674" s="3" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A675" s="4" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B675" s="3" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="676" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A676" s="4" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B676" s="3" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A677" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B677" s="3" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A678" s="4" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B678" s="3" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A679" s="4" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B679" s="3" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A680" s="4" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B680" s="3" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A681" s="4" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B681" s="3" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A682" s="4" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B682" s="3" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A683" s="4" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B683" s="3" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A684" s="4" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B684" s="3" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A685" s="4" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B685" s="3" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A686" s="4" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B686" s="3" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A687" s="4" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B687" s="3" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A688" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B688" s="3" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A689" s="4" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B689" s="3" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A690" s="4" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B690" s="3" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A691" s="4" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B691" s="3" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A692" s="4" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B692" s="3" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A693" s="4" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B693" s="3" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A694" s="4" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B694" s="3" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A695" s="4" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B695" s="3" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A696" s="4" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B696" s="3" t="s">
+        <v>1253</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
individually set sort type; support inherit of ares & phobos
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C69A96-3E77-4189-845A-5035BB0477A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FCE4BD-F1EA-4B1D-86BA-5AA389C0361D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9460" yWindow="3090" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="1334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="1354">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3704,9 +3704,6 @@
     <t>从地图文件夹重新读取资源文件</t>
   </si>
   <si>
-    <t>读取#include INI (Ares)</t>
-  </si>
-  <si>
     <t>编辑CSF触发参数时弹出CSF浏览器</t>
   </si>
   <si>
@@ -3716,9 +3713,6 @@
     <t>自动调整下拉菜单宽度</t>
   </si>
   <si>
-    <t>按名称而非ID排序触发/小队等</t>
-  </si>
-  <si>
     <t>编辑路径点参数时弹出下拉菜单</t>
   </si>
   <si>
@@ -4210,6 +4204,79 @@
   </si>
   <si>
     <t>读取单位art(md).ini中的Image= (Phobos)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SortByLabelName.Trigger</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序触发，覆盖全局设置</t>
+  </si>
+  <si>
+    <t>Options.SortByLabelName.Team</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序小队，覆盖全局设置</t>
+  </si>
+  <si>
+    <t>Options.SortByLabelName.Taskforce</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序特遣部队，覆盖全局设置</t>
+  </si>
+  <si>
+    <t>Options.SortByLabelName.Script</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序脚本，覆盖全局设置</t>
+  </si>
+  <si>
+    <t>Options.SortByLabelName.AITrigger</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按名称而非ID排序AI触发，覆盖全局设置</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序编辑器中的选中项</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.Search</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.NewTheaterType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置NewTheater类型 (Y = Ares, N = YR)</t>
+  </si>
+  <si>
+    <t>Options.AllowInherits</t>
+  </si>
+  <si>
+    <t>Options.IncludeType</t>
+  </si>
+  <si>
+    <t>设置包含类型 (Y = Phobos, N = Ares)</t>
+  </si>
+  <si>
+    <t>Options.InheritType</t>
+  </si>
+  <si>
+    <t>设置继承类型 (Y = Phobos, N = Ares)</t>
+  </si>
+  <si>
+    <t>读取#include INI (Ares/Phobos)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许读取继承的INI小节 (Ares/Phobos)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4597,10 +4664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D696"/>
+  <dimension ref="A1:D706"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A672" workbookViewId="0">
-      <selection activeCell="B631" sqref="B631"/>
+    <sheetView tabSelected="1" topLeftCell="A697" workbookViewId="0">
+      <selection activeCell="B707" sqref="B707"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -9545,7 +9612,7 @@
     </row>
     <row r="620" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A620" s="4" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="B620" s="3" t="s">
         <v>1180</v>
@@ -9553,7 +9620,7 @@
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A621" s="4" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="B621" s="3" t="s">
         <v>1181</v>
@@ -9561,7 +9628,7 @@
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622" s="4" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="B622" s="3" t="s">
         <v>1182</v>
@@ -9569,7 +9636,7 @@
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A623" s="4" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="B623" s="3" t="s">
         <v>1183</v>
@@ -9577,7 +9644,7 @@
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624" s="4" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="B624" s="3" t="s">
         <v>1184</v>
@@ -9585,7 +9652,7 @@
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A625" s="4" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="B625" s="3" t="s">
         <v>1185</v>
@@ -9593,7 +9660,7 @@
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A626" s="4" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="B626" s="3" t="s">
         <v>1186</v>
@@ -9601,7 +9668,7 @@
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A627" s="4" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="B627" s="3" t="s">
         <v>1187</v>
@@ -9609,7 +9676,7 @@
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A628" s="4" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="B628" s="3" t="s">
         <v>1188</v>
@@ -9617,7 +9684,7 @@
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A629" s="4" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="B629" s="3" t="s">
         <v>1189</v>
@@ -9625,7 +9692,7 @@
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A630" s="4" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="B630" s="3" t="s">
         <v>1190</v>
@@ -9633,534 +9700,614 @@
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A631" s="4" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="B631" s="3" t="s">
-        <v>1191</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A632" s="4" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="B632" s="3" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="C632" s="7"/>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A633" s="4" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="B633" s="3" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="C633" s="7"/>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A634" s="4" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="B634" s="3" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A635" s="4" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="B635" s="3" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A636" s="4" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="B636" s="3" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A637" s="4" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="B637" s="3" t="s">
-        <v>1195</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="638" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A638" s="4" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="B638" s="3" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="639" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A639" s="4" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="B639" s="3" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A640" s="4" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="B640" s="3" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A641" s="4" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="B641" s="3" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A642" s="4" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="B642" s="3" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A643" s="4" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="B643" s="3" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A644" s="4" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="B644" s="3" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A645" s="4" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="B645" s="3" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A646" s="4" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="B646" s="3" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A647" s="4" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="B647" s="3" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A648" s="4" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="B648" s="3" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A649" s="4" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="B649" s="3" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A650" s="4" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B650" s="3" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A651" s="4" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="B651" s="3" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A652" s="4" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="B652" s="3" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A653" s="4" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="B653" s="3" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A654" s="4" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="B654" s="3" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655" s="4" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="B655" s="3" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A656" s="4" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B656" s="3" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="657" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A657" s="4" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="B657" s="3" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="658" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A658" s="4" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="B658" s="3" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="659" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A659" s="4" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="B659" s="3" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="660" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A660" s="4" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="B660" s="3" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="661" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A661" s="4" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="B661" s="3" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="C661" s="7"/>
       <c r="D661" s="7"/>
     </row>
     <row r="662" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A662" s="4" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B662" s="3" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="663" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A663" s="4" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="B663" s="3" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="664" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A664" s="4" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="B664" s="3" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="665" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A665" s="4" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="B665" s="3" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="666" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A666" s="4" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="B666" s="3" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="667" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A667" s="4" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="B667" s="3" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="668" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A668" s="4" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="B668" s="3" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="669" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A669" s="4" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="B669" s="3" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="670" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A670" s="4" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="B670" s="3" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="671" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A671" s="4" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="B671" s="3" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="672" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A672" s="4" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="B672" s="3" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A673" s="4" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="B673" s="3" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A674" s="4" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="B674" s="3" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A675" s="4" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="B675" s="3" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A676" s="4" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="B676" s="3" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A677" s="4" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="B677" s="3" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A678" s="4" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="B678" s="3" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A679" s="4" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="B679" s="3" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A680" s="4" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="B680" s="3" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A681" s="4" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="B681" s="3" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A682" s="4" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B682" s="3" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A683" s="4" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="B683" s="3" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A684" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="B684" s="3" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A685" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="B685" s="3" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A686" s="4" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="B686" s="3" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A687" s="4" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="B687" s="3" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A688" s="4" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="B688" s="3" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A689" s="4" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="B689" s="3" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A690" s="4" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="B690" s="3" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A691" s="4" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="B691" s="3" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A692" s="4" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="B692" s="3" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A693" s="4" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="B693" s="3" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A694" s="4" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="B694" s="3" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A695" s="4" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="B695" s="3" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A696" s="4" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="B696" s="3" t="s">
-        <v>1253</v>
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A697" s="4" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B697" s="3" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A698" s="4" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B698" s="3" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A699" s="4" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B699" s="3" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A700" s="4" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B700" s="3" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A701" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B701" s="3" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="702" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A702" s="4" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B702" s="3" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A703" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B703" s="3" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A704" s="4" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B704" s="3" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A705" s="4" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B705" s="3" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A706" s="4" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B706" s="3" t="s">
+        <v>1351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support NewINIFormat5, rewrite copy & redo
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B9B5F3-AF90-4755-A0EB-8D08C49622F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2B65ED-A30F-4467-BF84-59B901179A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9460" yWindow="3090" windowWidth="28180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3690" yWindow="3940" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="1358">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4278,6 +4278,22 @@
   </si>
   <si>
     <t>设置单元格第一个步兵的位置(Y = 4, N = 0)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtOverlays</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用无限覆盖物 (Phobos)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MV_OverlayLimit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>覆盖物索引超过255，地图将以NewINIFormat=5保存。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4665,10 +4681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D706"/>
+  <dimension ref="A1:D708"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A664" workbookViewId="0">
-      <selection activeCell="D671" sqref="D671"/>
+    <sheetView tabSelected="1" topLeftCell="A697" workbookViewId="0">
+      <selection activeCell="B706" sqref="B706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10311,6 +10327,22 @@
         <v>1350</v>
       </c>
     </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A707" s="4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B707" s="3" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A708" s="4" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B708" s="3" t="s">
+        <v>1357</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix terrain custom palette bug, add LightingPreview.TintTileSetBrowserView
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2B65ED-A30F-4467-BF84-59B901179A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED6F27C-B410-46D0-8613-2B45A69405E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3690" yWindow="3940" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="1358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="1360">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4295,6 +4295,13 @@
   <si>
     <t>覆盖物索引超过255，地图将以NewINIFormat=5保存。</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.LightingPreview.TintTileSetBrowserView</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按照当前光照渲染地形浏览器图像</t>
   </si>
 </sst>
 </file>
@@ -4681,10 +4688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D708"/>
+  <dimension ref="A1:D709"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A697" workbookViewId="0">
-      <selection activeCell="B706" sqref="B706"/>
+    <sheetView tabSelected="1" topLeftCell="A643" workbookViewId="0">
+      <selection activeCell="B707" sqref="B707"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10343,6 +10350,14 @@
         <v>1357</v>
       </c>
     </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A709" s="4" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B709" s="3" t="s">
+        <v>1359</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add distance ruler func
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED6F27C-B410-46D0-8613-2B45A69405E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D03F12-BB47-4E8E-AA32-5A03E63CA2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3690" yWindow="3940" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="1360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="1368">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4243,10 +4243,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>搜索:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Options.NewTheaterType</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -4302,6 +4298,39 @@
   </si>
   <si>
     <t>按照当前光照渲染地形浏览器图像</t>
+  </si>
+  <si>
+    <t>搜索：</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.MapTools.DistanceRuler</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>距离标尺</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>距离: %s</t>
+  </si>
+  <si>
+    <t>XY: %d, %d, ΔXY: %d, %d</t>
+  </si>
+  <si>
+    <t>XY: %d, %d</t>
+  </si>
+  <si>
+    <t>DistanceRuler.InitCoordinate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DistanceRuler.Coordinate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DistanceRuler.Distance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4688,10 +4717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D709"/>
+  <dimension ref="A1:D713"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A643" workbookViewId="0">
-      <selection activeCell="B707" sqref="B707"/>
+    <sheetView tabSelected="1" topLeftCell="A683" workbookViewId="0">
+      <selection activeCell="A708" sqref="A708"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -9727,7 +9756,7 @@
         <v>1262</v>
       </c>
       <c r="B631" s="3" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.3">
@@ -10027,7 +10056,7 @@
         <v>1299</v>
       </c>
       <c r="B668" s="3" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="669" spans="1:4" x14ac:dyDescent="0.3">
@@ -10299,63 +10328,95 @@
         <v>1342</v>
       </c>
       <c r="B702" s="3" t="s">
-        <v>1343</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A703" s="4" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B703" s="3" t="s">
         <v>1344</v>
-      </c>
-      <c r="B703" s="3" t="s">
-        <v>1345</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A704" s="4" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="B704" s="3" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A705" s="4" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B705" s="3" t="s">
         <v>1347</v>
-      </c>
-      <c r="B705" s="3" t="s">
-        <v>1348</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A706" s="4" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B706" s="3" t="s">
         <v>1349</v>
-      </c>
-      <c r="B706" s="3" t="s">
-        <v>1350</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A707" s="4" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B707" s="3" t="s">
         <v>1354</v>
-      </c>
-      <c r="B707" s="3" t="s">
-        <v>1355</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A708" s="4" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B708" s="3" t="s">
         <v>1356</v>
-      </c>
-      <c r="B708" s="3" t="s">
-        <v>1357</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A709" s="4" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B709" s="3" t="s">
         <v>1358</v>
       </c>
-      <c r="B709" s="3" t="s">
-        <v>1359</v>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A710" s="4" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B710" s="3" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A711" s="4" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B711" s="3" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A712" s="4" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B712" s="3" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A713" s="4" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B713" s="3" t="s">
+        <v>1364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix resize map tube bug & keyboard related bugs
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB01DC7-ADEE-4DBD-AAE6-B76EFDEB63B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE21808-401C-4072-A738-CD2F1A9229DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3690" yWindow="3940" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="1368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="1370">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4330,6 +4330,13 @@
   </si>
   <si>
     <t>距离标尺\tCtrl+Shift+R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PressAToSwitchCliff</t>
+  </si>
+  <si>
+    <t>按A键以切换悬崖类型</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4717,10 +4724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D713"/>
+  <dimension ref="A1:D714"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A683" workbookViewId="0">
-      <selection activeCell="B710" sqref="B710"/>
+    <sheetView tabSelected="1" topLeftCell="A704" workbookViewId="0">
+      <selection activeCell="B712" sqref="B712"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10419,6 +10426,14 @@
         <v>1363</v>
       </c>
     </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A714" s="4" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B714" s="3" t="s">
+        <v>1369</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
save map can preserve existing sorting
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353FCB8E-1ED4-4134-8617-0D45D9327492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D97F9D-7D2B-416E-832F-061C9D05D0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2170" yWindow="3210" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2510" yWindow="3550" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,15 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="1378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="1382">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -3677,694 +3680,709 @@
     <t>局部变量过多</t>
   </si>
   <si>
+    <t>设置项</t>
+  </si>
+  <si>
+    <t>重新加载地图以应用此修改</t>
+  </si>
+  <si>
+    <t>重新启动FA2以应用此修改</t>
+  </si>
+  <si>
+    <t>屏蔽不可用所属方</t>
+  </si>
+  <si>
+    <t>将建筑按大小分类</t>
+  </si>
+  <si>
+    <t>在月球地图显示水面地形</t>
+  </si>
+  <si>
+    <t>加载平民建筑的额外翻译</t>
+  </si>
+  <si>
+    <t>从地图文件夹重新读取资源文件</t>
+  </si>
+  <si>
+    <t>编辑CSF触发参数时弹出CSF浏览器</t>
+  </si>
+  <si>
+    <t>复制触发/小队等时递增编号</t>
+  </si>
+  <si>
+    <t>自动调整下拉菜单宽度</t>
+  </si>
+  <si>
+    <t>编辑路径点参数时弹出下拉菜单</t>
+  </si>
+  <si>
+    <t>根据高度显示不同鼠标颜色</t>
+  </si>
+  <si>
+    <t>自动保存地图</t>
+  </si>
+  <si>
+    <t>仅以.map格式保存地图</t>
+  </si>
+  <si>
+    <t>生成更精细的多人游戏预览图</t>
+  </si>
+  <si>
+    <t>地图开头添加编码警告的注释</t>
+  </si>
+  <si>
+    <t>启用无限路径点 (Phobos)</t>
+  </si>
+  <si>
+    <t>启用无限变量 (Phobos)</t>
+  </si>
+  <si>
+    <t>按住shift放置地形时仅记录一次历史</t>
+  </si>
+  <si>
+    <t>按住shift放置覆盖图时仅记录一次历史</t>
+  </si>
+  <si>
+    <t>为路径点绘制矩形背景</t>
+  </si>
+  <si>
+    <t>为基地节点索引绘制矩形背景</t>
+  </si>
+  <si>
+    <t>将地形浏览器移至右侧</t>
+  </si>
+  <si>
+    <t>启用新的视觉样式(可能无法输入中文)</t>
+  </si>
+  <si>
+    <t>在随机树木窗口显示所有地形对象</t>
+  </si>
+  <si>
+    <t>在显存中分配DirectDraw surface</t>
+  </si>
+  <si>
+    <t>在DirectDrawCreate中使用emulation mode</t>
+  </si>
+  <si>
+    <t>使用双线性插值缩放绘图界面(更精细，但更卡)</t>
+  </si>
+  <si>
+    <t>使用独立服务器进程存储游戏素材</t>
+  </si>
+  <si>
+    <t>不将所属方翻译为其UIName</t>
+  </si>
+  <si>
+    <t>翻译所属方的同时显示英文原名</t>
+  </si>
+  <si>
+    <t>地图检查器的新检查仅弹出提示而非错误</t>
+  </si>
+  <si>
+    <t>地图检查器的INI长度限制为512而非128 (Ares)</t>
+  </si>
+  <si>
+    <t>加载素材启用严格NewTheater逻辑</t>
+  </si>
+  <si>
+    <t>禁止摆放重叠建筑</t>
+  </si>
+  <si>
+    <t>自动填写Upgrade数量</t>
+  </si>
+  <si>
+    <t>建筑存在Upgrade时设为满血</t>
+  </si>
+  <si>
+    <t>使用默认光照时调整单位RGB值</t>
+  </si>
+  <si>
+    <t>在小地图显示可视地图边界</t>
+  </si>
+  <si>
+    <t>编辑步兵时考虑鼠标位置</t>
+  </si>
+  <si>
+    <t>单元格只有单步兵时仍判断鼠标位置</t>
+  </si>
+  <si>
+    <t>拖拽步兵时考虑鼠标位置</t>
+  </si>
+  <si>
+    <t>放置步兵时考虑鼠标位置</t>
+  </si>
+  <si>
+    <t>固定中间步兵位置同InfantrySubCell.GameDefault</t>
+  </si>
+  <si>
+    <t>放置步兵时考虑地形对象占用</t>
+  </si>
+  <si>
+    <t>强制CString内存在堆上分配</t>
+  </si>
+  <si>
+    <t>启用严格错误捕获(会捕获C++ EH错误)</t>
+  </si>
+  <si>
+    <t>使用新的工具栏图标</t>
+  </si>
+  <si>
+    <t>不显示今日提示窗口</t>
+  </si>
+  <si>
+    <t>选择地形工具时不改变笔刷大小</t>
+  </si>
+  <si>
+    <t>放置地形时跳过隐藏单元格</t>
+  </si>
+  <si>
+    <t>在INI编辑器中忽略小队/特遣/脚本小节</t>
+  </si>
+  <si>
+    <t>ctrl填充地形时同时填充LAT</t>
+  </si>
+  <si>
+    <t>ctrl填充地形时将水面视为一类</t>
+  </si>
+  <si>
+    <t>加载并显示阴影</t>
+  </si>
+  <si>
+    <t>加载并显示可部署单位的更换图像</t>
+  </si>
+  <si>
+    <t>加载并显示水中单位的更换图像</t>
+  </si>
+  <si>
+    <t>加载并显示单位伤残的更换图像 (Phobos)</t>
+  </si>
+  <si>
+    <t>将悬浮单位渲染的更高</t>
+  </si>
+  <si>
+    <t>显示建筑物和地形对象的AlphaImage</t>
+  </si>
+  <si>
+    <t>将桥梁上单位渲染的更高</t>
+  </si>
+  <si>
+    <t>开启平面显示时隐藏地形ExtraImage</t>
+  </si>
+  <si>
+    <t>显示地图边界外的游戏对象</t>
+  </si>
+  <si>
+    <t>单位选项窗口显示&lt;Player @ X&gt;所属方 (Phobos)</t>
+  </si>
+  <si>
+    <t>检测地图文件的外部修改</t>
+  </si>
+  <si>
+    <t>计算武器射程时考虑悬崖影响</t>
+  </si>
+  <si>
+    <t>粘贴地形时默认显示描边</t>
+  </si>
+  <si>
+    <t>LocalVariablesExceed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalVariablesExceedTitle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.Options.Preferences</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.Label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ReloadMap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.Restart</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ObjectBrowser.SafeHouses</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ObjectBrowser.Foundation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.LoadLunarWater</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.LoadCivilianStringtable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ReloadGameFromMapFolder</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.AllowIncludes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.AllowPlusEqual</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ArtImageSwap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.TutorialTexts.Viewer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.CloneWithOrderedID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.AdjustDropdownWidth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SortByLabelName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SearchCombobox.Waypoint</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.CursorSelectionBound.AutoHeightColor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SaveMap.AutoSave</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SaveMap.OnlySaveMAP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SaveMap.BetterMapPreview</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SaveMap.FileEncodingComment</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtWaypoints</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtVariables</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.UndoRedo.ShiftPlaceTile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.UndoRedo.HoldPlaceOverlay</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.Waypoint.Background</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.BaseNodeIndex.Background</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.VerticalLayout</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.EnableVisualStyle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.RandomTerrainObjects</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.DDrawInVideoMem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.DDrawEmulation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.DDrawScalingBilinear</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.LoadImageDataFromServer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.NoHouseNameTranslation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.BetterHouseNameTranslation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtendedValidationNoError</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtendedValidationAres</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.HideNoRubbleBuilding</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.UseStrictNewTheater</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PlaceStructure.OverlappingCheck</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PlaceStructure.AutoUpgrade</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PlaceStructure.UpgradeStrength</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.LightingPreview.MultUnitColor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ShowMapBoundInMiniMap</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.GameDefault</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.Edit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.Edit.Single</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.Edit.Drag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.Edit.Place</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.Edit.FixCenter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InfantrySubCell.OccupationBits</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.StringBufferStackAllocation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.StrictExceptionFilter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.UseNewToolBarCameo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SkipTipsOfTheDay</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SkipBrushSizeChangeOnTools</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PlaceTileSkipHide</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.INIEditor.IgnoreTeams</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.FillArea.ConsiderLAT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.FillArea.ConsiderWater</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Shadow</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Deploy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Water</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Damage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Hover</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.AlphaImage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.InGameDisplay.Bridge</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.FlatToGroundHideExtra</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.DisplayObjectsOutside</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PlayerAtXForTechnos</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.FileWatcher</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.WeaponRangeBound.SubjectToElevation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.PasteShowOutline</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不渲染HP=0且LeaveRubble=no的建筑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取注册表小节的+= (Ares)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取单位art(md).ini中的Image= (Phobos)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SortByLabelName.Trigger</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序触发，覆盖全局设置</t>
+  </si>
+  <si>
+    <t>Options.SortByLabelName.Team</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序小队，覆盖全局设置</t>
+  </si>
+  <si>
+    <t>Options.SortByLabelName.Taskforce</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序特遣部队，覆盖全局设置</t>
+  </si>
+  <si>
+    <t>Options.SortByLabelName.Script</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序脚本，覆盖全局设置</t>
+  </si>
+  <si>
+    <t>Options.SortByLabelName.AITrigger</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按名称而非ID排序AI触发，覆盖全局设置</t>
+  </si>
+  <si>
+    <t>按名称而非ID排序编辑器中的选中项</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.Search</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.NewTheaterType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置NewTheater类型 (Y = Ares, N = YR)</t>
+  </si>
+  <si>
+    <t>Options.AllowInherits</t>
+  </si>
+  <si>
+    <t>Options.IncludeType</t>
+  </si>
+  <si>
+    <t>设置包含类型 (Y = Phobos, N = Ares)</t>
+  </si>
+  <si>
+    <t>Options.InheritType</t>
+  </si>
+  <si>
+    <t>设置继承类型 (Y = Phobos, N = Ares)</t>
+  </si>
+  <si>
+    <t>读取#include INI (Ares/Phobos)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许读取继承的INI小节 (Ares/Phobos)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置单元格第一个步兵的位置(Y = 4, N = 0)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtOverlays</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用无限覆盖物 (Phobos)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MV_OverlayLimit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>覆盖物索引超过255，地图将以NewINIFormat=5保存。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.LightingPreview.TintTileSetBrowserView</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按照当前光照渲染地形浏览器图像</t>
+  </si>
+  <si>
+    <t>搜索：</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Menu.MapTools.DistanceRuler</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>距离: %s</t>
+  </si>
+  <si>
+    <t>XY: %d, %d, ΔXY: %d, %d</t>
+  </si>
+  <si>
+    <t>XY: %d, %d</t>
+  </si>
+  <si>
+    <t>DistanceRuler.InitCoordinate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DistanceRuler.Coordinate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DistanceRuler.Distance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>距离标尺\tCtrl+Shift+R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PressAToSwitchCliff</t>
+  </si>
+  <si>
+    <t>按 A 键以切换悬崖类型</t>
+  </si>
+  <si>
+    <t>PressNumberToSwitchConnectedType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">按数字 %s 键以切换至 %s </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SwitchConnectedTypeIsWaterCliff</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(水上)</t>
+  </si>
+  <si>
+    <t>启用32向面向</t>
+  </si>
+  <si>
+    <t>启用32向拖拽</t>
+  </si>
+  <si>
+    <t>Options.ExtFacings.Drag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.ExtFacings</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.SaveMap.PreserveINISorting</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存时维持已有的ini小节顺序</t>
+  </si>
+  <si>
+    <t>偏好设置\tCtrl+Shift+P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Options.Title</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>偏好设置</t>
-  </si>
-  <si>
-    <t>设置项</t>
-  </si>
-  <si>
-    <t>重新加载地图以应用此修改</t>
-  </si>
-  <si>
-    <t>重新启动FA2以应用此修改</t>
-  </si>
-  <si>
-    <t>屏蔽不可用所属方</t>
-  </si>
-  <si>
-    <t>将建筑按大小分类</t>
-  </si>
-  <si>
-    <t>在月球地图显示水面地形</t>
-  </si>
-  <si>
-    <t>加载平民建筑的额外翻译</t>
-  </si>
-  <si>
-    <t>从地图文件夹重新读取资源文件</t>
-  </si>
-  <si>
-    <t>编辑CSF触发参数时弹出CSF浏览器</t>
-  </si>
-  <si>
-    <t>复制触发/小队等时递增编号</t>
-  </si>
-  <si>
-    <t>自动调整下拉菜单宽度</t>
-  </si>
-  <si>
-    <t>编辑路径点参数时弹出下拉菜单</t>
-  </si>
-  <si>
-    <t>根据高度显示不同鼠标颜色</t>
-  </si>
-  <si>
-    <t>自动保存地图</t>
-  </si>
-  <si>
-    <t>仅以.map格式保存地图</t>
-  </si>
-  <si>
-    <t>生成更精细的多人游戏预览图</t>
-  </si>
-  <si>
-    <t>地图开头添加编码警告的注释</t>
-  </si>
-  <si>
-    <t>启用无限路径点 (Phobos)</t>
-  </si>
-  <si>
-    <t>启用无限变量 (Phobos)</t>
-  </si>
-  <si>
-    <t>按住shift放置地形时仅记录一次历史</t>
-  </si>
-  <si>
-    <t>按住shift放置覆盖图时仅记录一次历史</t>
-  </si>
-  <si>
-    <t>为路径点绘制矩形背景</t>
-  </si>
-  <si>
-    <t>为基地节点索引绘制矩形背景</t>
-  </si>
-  <si>
-    <t>将地形浏览器移至右侧</t>
-  </si>
-  <si>
-    <t>启用新的视觉样式(可能无法输入中文)</t>
-  </si>
-  <si>
-    <t>在随机树木窗口显示所有地形对象</t>
-  </si>
-  <si>
-    <t>在显存中分配DirectDraw surface</t>
-  </si>
-  <si>
-    <t>在DirectDrawCreate中使用emulation mode</t>
-  </si>
-  <si>
-    <t>使用双线性插值缩放绘图界面(更精细，但更卡)</t>
-  </si>
-  <si>
-    <t>使用独立服务器进程存储游戏素材</t>
-  </si>
-  <si>
-    <t>不将所属方翻译为其UIName</t>
-  </si>
-  <si>
-    <t>翻译所属方的同时显示英文原名</t>
-  </si>
-  <si>
-    <t>地图检查器的新检查仅弹出提示而非错误</t>
-  </si>
-  <si>
-    <t>地图检查器的INI长度限制为512而非128 (Ares)</t>
-  </si>
-  <si>
-    <t>加载素材启用严格NewTheater逻辑</t>
-  </si>
-  <si>
-    <t>禁止摆放重叠建筑</t>
-  </si>
-  <si>
-    <t>自动填写Upgrade数量</t>
-  </si>
-  <si>
-    <t>建筑存在Upgrade时设为满血</t>
-  </si>
-  <si>
-    <t>使用默认光照时调整单位RGB值</t>
-  </si>
-  <si>
-    <t>在小地图显示可视地图边界</t>
-  </si>
-  <si>
-    <t>编辑步兵时考虑鼠标位置</t>
-  </si>
-  <si>
-    <t>单元格只有单步兵时仍判断鼠标位置</t>
-  </si>
-  <si>
-    <t>拖拽步兵时考虑鼠标位置</t>
-  </si>
-  <si>
-    <t>放置步兵时考虑鼠标位置</t>
-  </si>
-  <si>
-    <t>固定中间步兵位置同InfantrySubCell.GameDefault</t>
-  </si>
-  <si>
-    <t>放置步兵时考虑地形对象占用</t>
-  </si>
-  <si>
-    <t>强制CString内存在堆上分配</t>
-  </si>
-  <si>
-    <t>启用严格错误捕获(会捕获C++ EH错误)</t>
-  </si>
-  <si>
-    <t>使用新的工具栏图标</t>
-  </si>
-  <si>
-    <t>不显示今日提示窗口</t>
-  </si>
-  <si>
-    <t>选择地形工具时不改变笔刷大小</t>
-  </si>
-  <si>
-    <t>放置地形时跳过隐藏单元格</t>
-  </si>
-  <si>
-    <t>在INI编辑器中忽略小队/特遣/脚本小节</t>
-  </si>
-  <si>
-    <t>ctrl填充地形时同时填充LAT</t>
-  </si>
-  <si>
-    <t>ctrl填充地形时将水面视为一类</t>
-  </si>
-  <si>
-    <t>加载并显示阴影</t>
-  </si>
-  <si>
-    <t>加载并显示可部署单位的更换图像</t>
-  </si>
-  <si>
-    <t>加载并显示水中单位的更换图像</t>
-  </si>
-  <si>
-    <t>加载并显示单位伤残的更换图像 (Phobos)</t>
-  </si>
-  <si>
-    <t>将悬浮单位渲染的更高</t>
-  </si>
-  <si>
-    <t>显示建筑物和地形对象的AlphaImage</t>
-  </si>
-  <si>
-    <t>将桥梁上单位渲染的更高</t>
-  </si>
-  <si>
-    <t>开启平面显示时隐藏地形ExtraImage</t>
-  </si>
-  <si>
-    <t>显示地图边界外的游戏对象</t>
-  </si>
-  <si>
-    <t>单位选项窗口显示&lt;Player @ X&gt;所属方 (Phobos)</t>
-  </si>
-  <si>
-    <t>检测地图文件的外部修改</t>
-  </si>
-  <si>
-    <t>计算武器射程时考虑悬崖影响</t>
-  </si>
-  <si>
-    <t>粘贴地形时默认显示描边</t>
-  </si>
-  <si>
-    <t>LocalVariablesExceed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LocalVariablesExceedTitle</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Menu.Options.Preferences</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.Label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ReloadMap</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.Restart</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ObjectBrowser.SafeHouses</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ObjectBrowser.Foundation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.LoadLunarWater</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.LoadCivilianStringtable</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ReloadGameFromMapFolder</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.AllowIncludes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.AllowPlusEqual</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ArtImageSwap</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.TutorialTexts.Viewer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.CloneWithOrderedID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.AdjustDropdownWidth</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.SortByLabelName</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.SearchCombobox.Waypoint</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.CursorSelectionBound.AutoHeightColor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.SaveMap.AutoSave</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.SaveMap.OnlySaveMAP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.SaveMap.BetterMapPreview</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.SaveMap.FileEncodingComment</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ExtWaypoints</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ExtVariables</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.UndoRedo.ShiftPlaceTile</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.UndoRedo.HoldPlaceOverlay</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.Waypoint.Background</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.BaseNodeIndex.Background</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.VerticalLayout</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.EnableVisualStyle</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.RandomTerrainObjects</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.DDrawInVideoMem</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.DDrawEmulation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.DDrawScalingBilinear</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.LoadImageDataFromServer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.NoHouseNameTranslation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.BetterHouseNameTranslation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ExtendedValidationNoError</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ExtendedValidationAres</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.HideNoRubbleBuilding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.UseStrictNewTheater</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.PlaceStructure.OverlappingCheck</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.PlaceStructure.AutoUpgrade</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.PlaceStructure.UpgradeStrength</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.LightingPreview.MultUnitColor</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ShowMapBoundInMiniMap</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InfantrySubCell.GameDefault</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InfantrySubCell.Edit</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InfantrySubCell.Edit.Single</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InfantrySubCell.Edit.Drag</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InfantrySubCell.Edit.Place</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InfantrySubCell.Edit.FixCenter</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InfantrySubCell.OccupationBits</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.StringBufferStackAllocation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.StrictExceptionFilter</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.UseNewToolBarCameo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.SkipTipsOfTheDay</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.SkipBrushSizeChangeOnTools</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.PlaceTileSkipHide</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.INIEditor.IgnoreTeams</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.FillArea.ConsiderLAT</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.FillArea.ConsiderWater</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InGameDisplay.Shadow</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InGameDisplay.Deploy</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InGameDisplay.Water</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InGameDisplay.Damage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InGameDisplay.Hover</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InGameDisplay.AlphaImage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.InGameDisplay.Bridge</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.FlatToGroundHideExtra</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.DisplayObjectsOutside</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.PlayerAtXForTechnos</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.FileWatcher</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.WeaponRangeBound.SubjectToElevation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.PasteShowOutline</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>不渲染HP=0且LeaveRubble=no的建筑</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>读取注册表小节的+= (Ares)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>读取单位art(md).ini中的Image= (Phobos)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.SortByLabelName.Trigger</t>
-  </si>
-  <si>
-    <t>按名称而非ID排序触发，覆盖全局设置</t>
-  </si>
-  <si>
-    <t>Options.SortByLabelName.Team</t>
-  </si>
-  <si>
-    <t>按名称而非ID排序小队，覆盖全局设置</t>
-  </si>
-  <si>
-    <t>Options.SortByLabelName.Taskforce</t>
-  </si>
-  <si>
-    <t>按名称而非ID排序特遣部队，覆盖全局设置</t>
-  </si>
-  <si>
-    <t>Options.SortByLabelName.Script</t>
-  </si>
-  <si>
-    <t>按名称而非ID排序脚本，覆盖全局设置</t>
-  </si>
-  <si>
-    <t>Options.SortByLabelName.AITrigger</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>按名称而非ID排序AI触发，覆盖全局设置</t>
-  </si>
-  <si>
-    <t>按名称而非ID排序编辑器中的选中项</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.Search</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.NewTheaterType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置NewTheater类型 (Y = Ares, N = YR)</t>
-  </si>
-  <si>
-    <t>Options.AllowInherits</t>
-  </si>
-  <si>
-    <t>Options.IncludeType</t>
-  </si>
-  <si>
-    <t>设置包含类型 (Y = Phobos, N = Ares)</t>
-  </si>
-  <si>
-    <t>Options.InheritType</t>
-  </si>
-  <si>
-    <t>设置继承类型 (Y = Phobos, N = Ares)</t>
-  </si>
-  <si>
-    <t>读取#include INI (Ares/Phobos)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>允许读取继承的INI小节 (Ares/Phobos)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置单元格第一个步兵的位置(Y = 4, N = 0)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ExtOverlays</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>启用无限覆盖物 (Phobos)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MV_OverlayLimit</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>覆盖物索引超过255，地图将以NewINIFormat=5保存。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.LightingPreview.TintTileSetBrowserView</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>按照当前光照渲染地形浏览器图像</t>
-  </si>
-  <si>
-    <t>搜索：</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Menu.MapTools.DistanceRuler</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>距离: %s</t>
-  </si>
-  <si>
-    <t>XY: %d, %d, ΔXY: %d, %d</t>
-  </si>
-  <si>
-    <t>XY: %d, %d</t>
-  </si>
-  <si>
-    <t>DistanceRuler.InitCoordinate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DistanceRuler.Coordinate</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DistanceRuler.Distance</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>距离标尺\tCtrl+Shift+R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PressAToSwitchCliff</t>
-  </si>
-  <si>
-    <t>按 A 键以切换悬崖类型</t>
-  </si>
-  <si>
-    <t>PressNumberToSwitchConnectedType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">按数字 %s 键以切换至 %s </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SwitchConnectedTypeIsWaterCliff</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(水上)</t>
-  </si>
-  <si>
-    <t>启用32向面向</t>
-  </si>
-  <si>
-    <t>启用32向拖拽</t>
-  </si>
-  <si>
-    <t>Options.ExtFacings.Drag</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Options.ExtFacings</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4751,10 +4769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D718"/>
+  <dimension ref="A1:D720"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A704" workbookViewId="0">
-      <selection activeCell="B714" sqref="B714"/>
+    <sheetView tabSelected="1" topLeftCell="A709" workbookViewId="0">
+      <selection activeCell="D715" sqref="D715"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -9699,7 +9717,7 @@
     </row>
     <row r="620" spans="1:2" ht="35" x14ac:dyDescent="0.3">
       <c r="A620" s="4" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B620" s="3" t="s">
         <v>1180</v>
@@ -9707,7 +9725,7 @@
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A621" s="4" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B621" s="3" t="s">
         <v>1181</v>
@@ -9715,782 +9733,798 @@
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622" s="4" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B622" s="3" t="s">
-        <v>1182</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A623" s="4" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B623" s="3" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624" s="4" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B624" s="3" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A625" s="4" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B625" s="3" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A626" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B626" s="3" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A627" s="4" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B627" s="3" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A628" s="4" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B628" s="3" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A629" s="4" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B629" s="3" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A630" s="4" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B630" s="3" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A631" s="4" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B631" s="3" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A632" s="4" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B632" s="3" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="C632" s="7"/>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A633" s="4" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B633" s="3" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="C633" s="7"/>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A634" s="4" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B634" s="3" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A635" s="4" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B635" s="3" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A636" s="4" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B636" s="3" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A637" s="4" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B637" s="3" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="638" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A638" s="4" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B638" s="3" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="639" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A639" s="4" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B639" s="3" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A640" s="4" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="B640" s="3" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A641" s="4" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="B641" s="3" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A642" s="4" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B642" s="3" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A643" s="4" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B643" s="3" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A644" s="4" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B644" s="3" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A645" s="4" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B645" s="3" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A646" s="4" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B646" s="3" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A647" s="4" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B647" s="3" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A648" s="4" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B648" s="3" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A649" s="4" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B649" s="3" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A650" s="4" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="B650" s="3" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A651" s="4" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B651" s="3" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A652" s="4" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B652" s="3" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A653" s="4" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B653" s="3" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A654" s="4" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="B654" s="3" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655" s="4" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B655" s="3" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A656" s="4" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B656" s="3" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="657" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A657" s="4" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B657" s="3" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="658" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A658" s="4" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B658" s="3" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="659" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A659" s="4" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B659" s="3" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="660" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A660" s="4" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="B660" s="3" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="661" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A661" s="4" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B661" s="3" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="C661" s="7"/>
       <c r="D661" s="7"/>
     </row>
     <row r="662" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A662" s="4" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="B662" s="3" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="663" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A663" s="4" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="B663" s="3" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="664" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A664" s="4" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B664" s="3" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="665" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A665" s="4" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B665" s="3" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="666" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A666" s="4" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="B666" s="3" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="667" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A667" s="4" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="B667" s="3" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="668" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A668" s="4" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B668" s="3" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="669" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A669" s="4" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B669" s="3" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="670" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A670" s="4" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="B670" s="3" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="671" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A671" s="4" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="B671" s="3" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="672" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A672" s="4" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B672" s="3" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A673" s="4" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="B673" s="3" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A674" s="4" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B674" s="3" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A675" s="4" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B675" s="3" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A676" s="4" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="B676" s="3" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A677" s="4" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B677" s="3" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A678" s="4" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B678" s="3" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A679" s="4" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B679" s="3" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A680" s="4" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="B680" s="3" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A681" s="4" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B681" s="3" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A682" s="4" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="B682" s="3" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A683" s="4" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="B683" s="3" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A684" s="4" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="B684" s="3" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A685" s="4" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="B685" s="3" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A686" s="4" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="B686" s="3" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A687" s="4" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="B687" s="3" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A688" s="4" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="B688" s="3" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A689" s="4" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="B689" s="3" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A690" s="4" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="B690" s="3" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A691" s="4" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="B691" s="3" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A692" s="4" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B692" s="3" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A693" s="4" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="B693" s="3" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A694" s="4" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B694" s="3" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A695" s="4" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B695" s="3" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A696" s="4" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="B696" s="3" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A697" s="4" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B697" s="3" t="s">
         <v>1331</v>
-      </c>
-      <c r="B697" s="3" t="s">
-        <v>1332</v>
       </c>
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A698" s="4" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B698" s="3" t="s">
         <v>1333</v>
-      </c>
-      <c r="B698" s="3" t="s">
-        <v>1334</v>
       </c>
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A699" s="4" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B699" s="3" t="s">
         <v>1335</v>
-      </c>
-      <c r="B699" s="3" t="s">
-        <v>1336</v>
       </c>
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A700" s="4" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B700" s="3" t="s">
         <v>1337</v>
-      </c>
-      <c r="B700" s="3" t="s">
-        <v>1338</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A701" s="4" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B701" s="3" t="s">
         <v>1339</v>
-      </c>
-      <c r="B701" s="3" t="s">
-        <v>1340</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A702" s="4" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B702" s="3" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A703" s="4" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B703" s="3" t="s">
         <v>1343</v>
-      </c>
-      <c r="B703" s="3" t="s">
-        <v>1344</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A704" s="4" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B704" s="3" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A705" s="4" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B705" s="3" t="s">
         <v>1346</v>
-      </c>
-      <c r="B705" s="3" t="s">
-        <v>1347</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A706" s="4" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B706" s="3" t="s">
         <v>1348</v>
-      </c>
-      <c r="B706" s="3" t="s">
-        <v>1349</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A707" s="4" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B707" s="3" t="s">
         <v>1353</v>
-      </c>
-      <c r="B707" s="3" t="s">
-        <v>1354</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A708" s="4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B708" s="3" t="s">
         <v>1355</v>
-      </c>
-      <c r="B708" s="3" t="s">
-        <v>1356</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A709" s="4" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B709" s="3" t="s">
         <v>1357</v>
-      </c>
-      <c r="B709" s="3" t="s">
-        <v>1358</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A710" s="4" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="B710" s="3" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A711" s="4" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="B711" s="3" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A712" s="4" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="B712" s="3" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A713" s="4" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="B713" s="3" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A714" s="4" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B714" s="3" t="s">
         <v>1368</v>
-      </c>
-      <c r="B714" s="3" t="s">
-        <v>1369</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A715" s="4" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B715" s="3" t="s">
         <v>1370</v>
-      </c>
-      <c r="B715" s="3" t="s">
-        <v>1371</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A716" s="4" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B716" s="3" t="s">
         <v>1372</v>
-      </c>
-      <c r="B716" s="3" t="s">
-        <v>1373</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A717" s="4" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B717" s="3" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A718" s="4" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="B718" s="3" t="s">
-        <v>1375</v>
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A719" s="4" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B719" s="3" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A720" s="4" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B720" s="3" t="s">
+        <v>1381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
undo redo for all objects
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D97F9D-7D2B-416E-832F-061C9D05D0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27BDEBE-5C39-4917-8CEF-19B381C59389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2510" yWindow="3550" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="1382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="1384">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4383,6 +4383,13 @@
   </si>
   <si>
     <t>偏好设置</t>
+  </si>
+  <si>
+    <t>Options.UndoRedo.RecordObjects</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>记录游戏对象修改历史</t>
   </si>
 </sst>
 </file>
@@ -4769,10 +4776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D720"/>
+  <dimension ref="A1:D721"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A709" workbookViewId="0">
-      <selection activeCell="D715" sqref="D715"/>
+      <selection activeCell="B719" sqref="B719"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10527,6 +10534,14 @@
         <v>1381</v>
       </c>
     </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A721" s="4" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B721" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix some bugs in ext mix loader
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D612E642-4B52-4E41-ADEE-82CD54452FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18033E1-9830-4F6B-9E27-72FBF04D4183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2510" yWindow="3550" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="1384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="1386">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4390,6 +4390,13 @@
   </si>
   <si>
     <t>按住shift放置覆盖物时仅记录一次历史</t>
+  </si>
+  <si>
+    <t>Options.ExtMixLoader</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用新的Mix加载方式</t>
   </si>
 </sst>
 </file>
@@ -4776,10 +4783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D721"/>
+  <dimension ref="A1:D722"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="B215" sqref="B215"/>
+    <sheetView tabSelected="1" topLeftCell="A710" workbookViewId="0">
+      <selection activeCell="B718" sqref="B718"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10542,6 +10549,14 @@
         <v>1370</v>
       </c>
     </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A722" s="4" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B722" s="3" t="s">
+        <v>1385</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support 3x3REFINERY & drag facing preview
</commit_message>
<xml_diff>
--- a/Supplementary/文档/FALanguage新增标签.xlsx
+++ b/Supplementary/文档/FALanguage新增标签.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\YURI\源码\FA2spHDM\Supplementary\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CB651F-F07B-4D18-8A7D-BEBF58CC3B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207E5766-F065-4AA4-BA54-74FD8411B1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2510" yWindow="3550" windowWidth="28080" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="1390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="1392">
   <si>
     <t>INIEditorTitle</t>
   </si>
@@ -4411,6 +4411,13 @@
   </si>
   <si>
     <t>单击以绘制隧道，双击以设置终点并完成编辑。隧道长度不能超过100。</t>
+  </si>
+  <si>
+    <t>Options.ExtFacings.DragPreview</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>拖拽面向时实时预览</t>
   </si>
 </sst>
 </file>
@@ -4792,10 +4799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D724"/>
+  <dimension ref="A1:D725"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A706" workbookViewId="0">
-      <selection activeCell="B710" sqref="B710"/>
+      <selection activeCell="B720" sqref="B720"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -10582,6 +10589,14 @@
         <v>1389</v>
       </c>
     </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A725" s="2" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B725" s="2" t="s">
+        <v>1391</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>